<commit_message>
added paper link + added motor schematic
</commit_message>
<xml_diff>
--- a/Generator/2dparts_schematic_materials-gen.xlsx
+++ b/Generator/2dparts_schematic_materials-gen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\school\2ndyr\1stsem\emag\generotr\Generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{855A2FF0-F1D9-4259-A591-95193CF2BBB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{139083B3-6BC9-41B6-94A4-818743CB9452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6EB7C18F-EE50-4A76-837B-874021D0598F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{6EB7C18F-EE50-4A76-837B-874021D0598F}"/>
   </bookViews>
   <sheets>
     <sheet name="General Schematic" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>Yellow box:</t>
   </si>
@@ -41,6 +41,12 @@
   </si>
   <si>
     <t>wala kakalikutin</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>S</t>
   </si>
 </sst>
 </file>
@@ -448,8 +454,13 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="en-PH" sz="1100"/>
-            <a:t>6.8 Ah + 3Ah</a:t>
+            <a:t>3</a:t>
           </a:r>
+          <a:r>
+            <a:rPr lang="en-PH" sz="1100" baseline="0"/>
+            <a:t> Ah</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-PH" sz="1100"/>
         </a:p>
         <a:p>
           <a:pPr algn="l"/>
@@ -473,16 +484,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>99060</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>79</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
+      <xdr:rowOff>22860</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>487680</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>388620</xdr:colOff>
       <xdr:row>83</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:rowOff>144780</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -497,7 +508,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3756660" y="14790420"/>
+          <a:off x="4480560" y="6972300"/>
           <a:ext cx="998220" cy="853440"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -774,16 +785,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>341494</xdr:colOff>
-      <xdr:row>83</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>388620</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>121920</xdr:colOff>
-      <xdr:row>83</xdr:row>
-      <xdr:rowOff>12177</xdr:rowOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -795,13 +806,13 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
-          <a:endCxn id="17" idx="5"/>
+          <a:endCxn id="17" idx="6"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="4608694" y="15514320"/>
-          <a:ext cx="999626" cy="4557"/>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="5478780" y="7399020"/>
+          <a:ext cx="342900" cy="15240"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -826,16 +837,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>541020</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>236220</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>22860</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
+      <xdr:rowOff>7620</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -847,13 +858,14 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
+          <a:stCxn id="74" idx="3"/>
           <a:endCxn id="10" idx="1"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="4198620" y="10210800"/>
-          <a:ext cx="701040" cy="15240"/>
+        <a:xfrm>
+          <a:off x="2887980" y="2354580"/>
+          <a:ext cx="2225040" cy="30480"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -878,16 +890,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>205740</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>213360</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>121920</xdr:rowOff>
+      <xdr:rowOff>144780</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>45720</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>144780</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -901,9 +913,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3863340" y="9959340"/>
-          <a:ext cx="1059180" cy="22860"/>
+        <a:xfrm flipV="1">
+          <a:off x="2865120" y="2156460"/>
+          <a:ext cx="2270760" cy="7620"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -981,16 +993,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>82</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>274320</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>586740</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>327660</xdr:colOff>
       <xdr:row>96</xdr:row>
-      <xdr:rowOff>45720</xdr:rowOff>
+      <xdr:rowOff>83820</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1005,8 +1017,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1143000" y="15499080"/>
-          <a:ext cx="2491740" cy="2430780"/>
+          <a:off x="274320" y="7711440"/>
+          <a:ext cx="2705100" cy="2430780"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -1142,8 +1154,8 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>563880</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>350520</xdr:colOff>
       <xdr:row>85</xdr:row>
       <xdr:rowOff>137160</xdr:rowOff>
     </xdr:from>
@@ -1166,8 +1178,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="3611880" y="16009620"/>
-          <a:ext cx="2293620" cy="68580"/>
+          <a:off x="3002280" y="8183880"/>
+          <a:ext cx="3116580" cy="68580"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1192,16 +1204,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>106680</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>464820</xdr:colOff>
       <xdr:row>67</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>129540</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>137160</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>464820</xdr:colOff>
       <xdr:row>72</xdr:row>
-      <xdr:rowOff>53340</xdr:rowOff>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1215,9 +1227,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="1325880" y="12733020"/>
-          <a:ext cx="30480" cy="815340"/>
+        <a:xfrm>
+          <a:off x="1074420" y="4884420"/>
+          <a:ext cx="0" cy="861060"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1242,16 +1254,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>354330</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>167640</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>255270</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>365760</xdr:colOff>
-      <xdr:row>71</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1268,7 +1280,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="1573530" y="12931140"/>
+          <a:off x="2907030" y="5151120"/>
           <a:ext cx="11430" cy="556260"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1294,16 +1306,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>441960</xdr:colOff>
-      <xdr:row>72</xdr:row>
-      <xdr:rowOff>129540</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>106680</xdr:colOff>
-      <xdr:row>75</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>289560</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1318,7 +1330,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10805160" y="13624560"/>
+          <a:off x="9982200" y="5623560"/>
           <a:ext cx="883920" cy="556260"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
@@ -1373,15 +1385,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>518160</xdr:colOff>
-      <xdr:row>75</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>274320</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
       <xdr:row>75</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:rowOff>15240</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1398,8 +1410,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="6004560" y="14180820"/>
-          <a:ext cx="5242560" cy="0"/>
+          <a:off x="6233160" y="6179820"/>
+          <a:ext cx="4191000" cy="53340"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1432,8 +1444,8 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>129540</xdr:colOff>
-      <xdr:row>83</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1448,8 +1460,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="5600700" y="13136880"/>
-          <a:ext cx="15240" cy="2377440"/>
+          <a:off x="5814060" y="5311140"/>
+          <a:ext cx="15240" cy="2087880"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1533,9 +1545,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>75</xdr:row>
-      <xdr:rowOff>160020</xdr:rowOff>
+      <xdr:colOff>541020</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1549,9 +1561,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="6019800" y="13159740"/>
-          <a:ext cx="0" cy="1043940"/>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="6233160" y="5334000"/>
+          <a:ext cx="7620" cy="876300"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1576,16 +1588,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>71</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>601980</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>403860</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
       <xdr:row>74</xdr:row>
-      <xdr:rowOff>129540</xdr:rowOff>
+      <xdr:rowOff>175260</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1600,8 +1612,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="914400" y="13487400"/>
-          <a:ext cx="1318260" cy="502920"/>
+          <a:off x="2034540" y="5707380"/>
+          <a:ext cx="1531620" cy="502920"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -1641,7 +1653,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-PH" sz="1100" baseline="0"/>
-            <a:t>5v; 5-6A</a:t>
+            <a:t>5v; max 5-6A</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-PH" sz="1100"/>
@@ -1654,16 +1666,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>487680</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>716280</xdr:colOff>
       <xdr:row>74</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>175260</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>601980</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>731520</xdr:colOff>
       <xdr:row>83</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1678,8 +1690,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2926080" y="13860780"/>
-          <a:ext cx="114300" cy="1722120"/>
+          <a:off x="1325880" y="6210300"/>
+          <a:ext cx="15240" cy="1562100"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1704,16 +1716,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>251460</xdr:colOff>
-      <xdr:row>73</xdr:row>
-      <xdr:rowOff>45720</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>434340</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>510540</xdr:colOff>
       <xdr:row>83</xdr:row>
-      <xdr:rowOff>60960</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1728,8 +1740,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2689860" y="13723620"/>
-          <a:ext cx="91440" cy="1844040"/>
+          <a:off x="1043940" y="6088380"/>
+          <a:ext cx="76200" cy="1744980"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1754,16 +1766,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>403860</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
       <xdr:row>73</xdr:row>
-      <xdr:rowOff>60960</xdr:rowOff>
+      <xdr:rowOff>49530</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>441960</xdr:colOff>
-      <xdr:row>74</xdr:row>
-      <xdr:rowOff>41910</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1780,9 +1792,9 @@
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2232660" y="13738860"/>
-          <a:ext cx="8572500" cy="163830"/>
+        <a:xfrm flipV="1">
+          <a:off x="3566160" y="5901690"/>
+          <a:ext cx="6416040" cy="57150"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1807,16 +1819,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>598170</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>499110</xdr:colOff>
       <xdr:row>73</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>510540</xdr:colOff>
       <xdr:row>79</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
+      <xdr:rowOff>22860</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1833,8 +1845,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="4255770" y="13769340"/>
-          <a:ext cx="11430" cy="1021080"/>
+          <a:off x="4979670" y="5928360"/>
+          <a:ext cx="11430" cy="1043940"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1860,15 +1872,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>358140</xdr:colOff>
+      <xdr:colOff>274320</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>30480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>365760</xdr:colOff>
+      <xdr:colOff>289560</xdr:colOff>
       <xdr:row>73</xdr:row>
-      <xdr:rowOff>129540</xdr:rowOff>
+      <xdr:rowOff>99060</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1883,8 +1895,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5234940" y="13167360"/>
-          <a:ext cx="7620" cy="640080"/>
+          <a:off x="5364480" y="5334000"/>
+          <a:ext cx="15240" cy="617220"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1909,16 +1921,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>320040</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
       <xdr:row>74</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
+      <xdr:rowOff>7620</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>449580</xdr:colOff>
-      <xdr:row>75</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>22860</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1932,59 +1944,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2148840" y="13876020"/>
-          <a:ext cx="8663940" cy="167640"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>140970</xdr:colOff>
-      <xdr:row>74</xdr:row>
-      <xdr:rowOff>60960</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>79</xdr:row>
-      <xdr:rowOff>167640</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="116" name="Straight Connector 115">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F77037C-6222-3D4E-2A5C-3DA09FD452C3}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="4408170" y="13921740"/>
-          <a:ext cx="11430" cy="1021080"/>
+        <a:xfrm flipV="1">
+          <a:off x="3566160" y="6042660"/>
+          <a:ext cx="6423660" cy="38100"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2010,15 +1972,65 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>510540</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>106680</xdr:rowOff>
+      <xdr:colOff>53340</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>518160</xdr:colOff>
+      <xdr:colOff>68580</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="116" name="Straight Connector 115">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F77037C-6222-3D4E-2A5C-3DA09FD452C3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="5143500" y="6080760"/>
+          <a:ext cx="15240" cy="952500"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>403860</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>434340</xdr:colOff>
       <xdr:row>74</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>68580</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2032,9 +2044,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="5387340" y="13053060"/>
-          <a:ext cx="7620" cy="883920"/>
+        <a:xfrm>
+          <a:off x="5494020" y="5349240"/>
+          <a:ext cx="30480" cy="754380"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2124,23 +2136,75 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>61</xdr:row>
-      <xdr:rowOff>160020</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>373380</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>579120</xdr:colOff>
-      <xdr:row>61</xdr:row>
-      <xdr:rowOff>160020</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>403860</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="135" name="Straight Connector 134">
+        <xdr:cNvPr id="146" name="Straight Connector 145">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5130711-FF85-4C7A-72E1-D60ABB8B7844}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F3C9B9A-EB03-4875-884D-1AA80A0CB0BA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="14" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1805940" y="4145280"/>
+          <a:ext cx="30480" cy="800100"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>586740</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>594360</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="147" name="Straight Connector 146">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E881FCF-DBEE-68AB-33C1-C76E1D82A2D8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2148,8 +2212,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2514600" y="11643360"/>
-          <a:ext cx="1722120" cy="0"/>
+          <a:off x="2019300" y="4160520"/>
+          <a:ext cx="7620" cy="1028700"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2174,23 +2238,73 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>259080</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>106680</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>708660</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>274320</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>144780</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>297180</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="138" name="Straight Connector 137">
+        <xdr:cNvPr id="150" name="Straight Connector 149">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{91F208B4-88A3-2B50-0EFF-EAC0B187F143}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{646D462F-BCB9-08E3-9B63-732CDC26509E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1318260" y="5143500"/>
+          <a:ext cx="1630680" cy="15240"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>449580</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>129540</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="151" name="Straight Connector 150">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD21FA15-2251-82FE-2700-D1B412CDB6B8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2198,8 +2312,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3916680" y="9944100"/>
-          <a:ext cx="15240" cy="1501140"/>
+          <a:off x="1059180" y="4876800"/>
+          <a:ext cx="1722120" cy="30480"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2224,32 +2338,260 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>320040</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rectangle: Rounded Corners 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{321C48DB-C23F-731C-DF18-CC9F904DC7ED}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="320040" y="5730240"/>
+          <a:ext cx="1531620" cy="502920"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent4">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-PH" sz="1100"/>
+            <a:t>buck converter</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-PH" sz="1100"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-PH" sz="1100"/>
+            <a:t>(output: </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-PH" sz="1100" baseline="0"/>
+            <a:t>5v; max 5-6A</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-PH" sz="1100"/>
+            <a:t>)</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>83820</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>297180</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>160020</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="140" name="Straight Connector 139">
+        <xdr:cNvPr id="6" name="Straight Connector 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F62E83B-154C-BA74-FC0F-B0001A461443}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79D52673-6F2C-1C5E-F66F-883DEF6AD3BE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="2522220" y="11452860"/>
-          <a:ext cx="1432560" cy="7620"/>
+        <a:xfrm flipH="1">
+          <a:off x="2735580" y="4899660"/>
+          <a:ext cx="30480" cy="815340"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>681990</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>693420</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Straight Connector 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D55E1D2-2AA6-4157-8B2D-959D87A64EFE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1291590" y="5173980"/>
+          <a:ext cx="11430" cy="556260"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>701040</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>53340</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="50" name="Straight Connector 49">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{593E1216-AFD5-8D4D-360C-A06202A9EF62}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1310640" y="7040880"/>
+          <a:ext cx="2613660" cy="38100"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>472440</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>487680</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="56" name="Straight Connector 55">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FAFF5D1-E8F1-56DC-A70D-6BA961F6ECD6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1082040" y="6896100"/>
+          <a:ext cx="2667000" cy="15240"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2275,31 +2617,31 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>167640</xdr:rowOff>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>556260</xdr:colOff>
-      <xdr:row>62</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:colOff>60960</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="143" name="Straight Connector 142">
+        <xdr:cNvPr id="59" name="Straight Connector 58">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E959FC38-5F7D-2F04-9670-151CC55915FC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{35681589-ABD8-F16A-ED74-FA7219FCF543}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="4210050" y="10187940"/>
-          <a:ext cx="3810" cy="1485900"/>
+        <a:xfrm>
+          <a:off x="3909060" y="6080760"/>
+          <a:ext cx="22860" cy="982980"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2324,23 +2666,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>281940</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>144780</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>449580</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="146" name="Straight Connector 145">
+        <xdr:cNvPr id="60" name="Straight Connector 59">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F3C9B9A-EB03-4875-884D-1AA80A0CB0BA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{71800C2A-FA7C-A154-68BA-2F783FB1F9BA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2348,8 +2690,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3939540" y="11445240"/>
-          <a:ext cx="7620" cy="1318260"/>
+          <a:off x="3710940" y="5958840"/>
+          <a:ext cx="7620" cy="937260"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2374,152 +2716,3198 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>61</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>358140</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>548640</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>53340</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>236220</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="147" name="Straight Connector 146">
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="74" name="Rectangle: Rounded Corners 73">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E881FCF-DBEE-68AB-33C1-C76E1D82A2D8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D3D0609-F3AD-2BFD-2C99-7EB4CF829EAC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="4191000" y="11597640"/>
-          <a:ext cx="15240" cy="1402080"/>
+        <a:xfrm>
+          <a:off x="967740" y="1973580"/>
+          <a:ext cx="1920240" cy="762000"/>
         </a:xfrm>
-        <a:prstGeom prst="line">
+        <a:prstGeom prst="roundRect">
           <a:avLst/>
         </a:prstGeom>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="dk1"/>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent4">
+            <a:shade val="15000"/>
+          </a:schemeClr>
         </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent4"/>
         </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="dk1"/>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent4"/>
         </a:effectRef>
         <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
+          <a:schemeClr val="lt1"/>
         </a:fontRef>
       </xdr:style>
-    </xdr:cxnSp>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-PH" sz="1100"/>
+            <a:t>battery 7.4 (8.1v max</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-PH" sz="1100" baseline="0"/>
+            <a:t> reality</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-PH" sz="1100"/>
+            <a:t>) output</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-PH" sz="1100"/>
+            <a:t>6.8</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-PH" sz="1100" baseline="0"/>
+            <a:t> Ah (2S)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-PH" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-PH" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-PH" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-PH" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>257695</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>157941</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>135775</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>8312</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Oval 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07654E69-2DC0-34CB-DBA9-B4C58FC5D469}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7572895" y="6143105"/>
+          <a:ext cx="1706880" cy="1651462"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-PH" sz="1100" b="0" cap="none" spc="0">
+              <a:ln w="0"/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="38100" dist="19050" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:schemeClr val="dk1">
+                    <a:alpha val="40000"/>
+                  </a:schemeClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>shaft 8cm</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-PH" sz="1100" b="0" cap="none" spc="0" baseline="0">
+              <a:ln w="0"/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="38100" dist="19050" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:schemeClr val="dk1">
+                    <a:alpha val="40000"/>
+                  </a:schemeClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </a:rPr>
+            <a:t> diameter</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-PH" sz="1100" b="0" cap="none" spc="0">
+            <a:ln w="0"/>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst>
+              <a:outerShdw blurRad="38100" dist="19050" dir="2700000" algn="tl" rotWithShape="0">
+                <a:schemeClr val="dk1">
+                  <a:alpha val="40000"/>
+                </a:schemeClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>350520</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>581891</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>138546</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>595745</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>152401</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="150" name="Straight Connector 149">
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{646D462F-BCB9-08E3-9B63-732CDC26509E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E35A43EA-707C-757F-1445-5A11DDBD20A8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1783080" y="5120640"/>
-          <a:ext cx="2621280" cy="7620"/>
+          <a:off x="7897091" y="5403273"/>
+          <a:ext cx="1233054" cy="374073"/>
         </a:xfrm>
-        <a:prstGeom prst="line">
+        <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="dk1"/>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
         </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
         </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="dk1"/>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
         </a:effectRef>
         <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
+          <a:schemeClr val="lt1"/>
         </a:fontRef>
       </xdr:style>
-    </xdr:cxnSp>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-PH" sz="1100"/>
+            <a:t>mmagnet</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-PH" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>99060</xdr:colOff>
-      <xdr:row>67</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>540328</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>166254</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>297180</xdr:colOff>
-      <xdr:row>67</xdr:row>
-      <xdr:rowOff>160020</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>554182</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="151" name="Straight Connector 150">
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rectangle 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD21FA15-2251-82FE-2700-D1B412CDB6B8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A783567-AF56-B244-3B2B-E42EA10A6A5E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
       <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="1318260" y="12733020"/>
-          <a:ext cx="2636520" cy="7620"/>
+        <a:xfrm>
+          <a:off x="7855528" y="8132618"/>
+          <a:ext cx="1233054" cy="374073"/>
         </a:xfrm>
-        <a:prstGeom prst="line">
+        <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="accent2"/>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
         </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent2"/>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
         </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent2"/>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
         </a:effectRef>
         <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
+          <a:schemeClr val="lt1"/>
         </a:fontRef>
       </xdr:style>
-    </xdr:cxnSp>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-PH" sz="1100"/>
+            <a:t>magnet</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>138546</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>166256</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>512619</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>138547</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Rectangle 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70961756-FF25-00A9-F783-08A2D96D71F8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="9462656" y="6761019"/>
+          <a:ext cx="1233054" cy="374073"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-PH" sz="1100"/>
+            <a:t>magnet</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>124692</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>27713</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>498765</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>4</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Rectangle 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D297B252-4B97-44FC-7009-B105ADF68595}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="6400802" y="6802585"/>
+          <a:ext cx="1233054" cy="374073"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-PH" sz="1100"/>
+            <a:t>magnet</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>561677</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>150777</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>518160</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>154531</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Freeform: Shape 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE8598B5-4AF3-F1D8-4D09-DA55D2260BE8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6657677" y="1272995"/>
+          <a:ext cx="3614083" cy="2705391"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="connsiteX0" fmla="*/ 3220614 w 3614083"/>
+            <a:gd name="connsiteY0" fmla="*/ 417259 h 2705391"/>
+            <a:gd name="connsiteX1" fmla="*/ 3137487 w 3614083"/>
+            <a:gd name="connsiteY1" fmla="*/ 361841 h 2705391"/>
+            <a:gd name="connsiteX2" fmla="*/ 2139959 w 3614083"/>
+            <a:gd name="connsiteY2" fmla="*/ 209441 h 2705391"/>
+            <a:gd name="connsiteX3" fmla="*/ 1627341 w 3614083"/>
+            <a:gd name="connsiteY3" fmla="*/ 1511768 h 2705391"/>
+            <a:gd name="connsiteX4" fmla="*/ 2236941 w 3614083"/>
+            <a:gd name="connsiteY4" fmla="*/ 2661695 h 2705391"/>
+            <a:gd name="connsiteX5" fmla="*/ 3123632 w 3614083"/>
+            <a:gd name="connsiteY5" fmla="*/ 2689404 h 2705391"/>
+            <a:gd name="connsiteX6" fmla="*/ 3386868 w 3614083"/>
+            <a:gd name="connsiteY6" fmla="*/ 1664168 h 2705391"/>
+            <a:gd name="connsiteX7" fmla="*/ 2638723 w 3614083"/>
+            <a:gd name="connsiteY7" fmla="*/ 458823 h 2705391"/>
+            <a:gd name="connsiteX8" fmla="*/ 1932141 w 3614083"/>
+            <a:gd name="connsiteY8" fmla="*/ 389550 h 2705391"/>
+            <a:gd name="connsiteX9" fmla="*/ 1655050 w 3614083"/>
+            <a:gd name="connsiteY9" fmla="*/ 735914 h 2705391"/>
+            <a:gd name="connsiteX10" fmla="*/ 1904432 w 3614083"/>
+            <a:gd name="connsiteY10" fmla="*/ 1442495 h 2705391"/>
+            <a:gd name="connsiteX11" fmla="*/ 2292359 w 3614083"/>
+            <a:gd name="connsiteY11" fmla="*/ 1622604 h 2705391"/>
+            <a:gd name="connsiteX12" fmla="*/ 3040505 w 3614083"/>
+            <a:gd name="connsiteY12" fmla="*/ 1678023 h 2705391"/>
+            <a:gd name="connsiteX13" fmla="*/ 3165196 w 3614083"/>
+            <a:gd name="connsiteY13" fmla="*/ 223295 h 2705391"/>
+            <a:gd name="connsiteX14" fmla="*/ 2139959 w 3614083"/>
+            <a:gd name="connsiteY14" fmla="*/ 98604 h 2705391"/>
+            <a:gd name="connsiteX15" fmla="*/ 796068 w 3614083"/>
+            <a:gd name="connsiteY15" fmla="*/ 528095 h 2705391"/>
+            <a:gd name="connsiteX16" fmla="*/ 200323 w 3614083"/>
+            <a:gd name="connsiteY16" fmla="*/ 1123841 h 2705391"/>
+            <a:gd name="connsiteX17" fmla="*/ 2112250 w 3614083"/>
+            <a:gd name="connsiteY17" fmla="*/ 2398459 h 2705391"/>
+            <a:gd name="connsiteX18" fmla="*/ 2888105 w 3614083"/>
+            <a:gd name="connsiteY18" fmla="*/ 2384604 h 2705391"/>
+            <a:gd name="connsiteX19" fmla="*/ 3331450 w 3614083"/>
+            <a:gd name="connsiteY19" fmla="*/ 1290095 h 2705391"/>
+            <a:gd name="connsiteX20" fmla="*/ 3179050 w 3614083"/>
+            <a:gd name="connsiteY20" fmla="*/ 361841 h 2705391"/>
+            <a:gd name="connsiteX21" fmla="*/ 712941 w 3614083"/>
+            <a:gd name="connsiteY21" fmla="*/ 264859 h 2705391"/>
+            <a:gd name="connsiteX22" fmla="*/ 61777 w 3614083"/>
+            <a:gd name="connsiteY22" fmla="*/ 888314 h 2705391"/>
+            <a:gd name="connsiteX23" fmla="*/ 131050 w 3614083"/>
+            <a:gd name="connsiteY23" fmla="*/ 1567186 h 2705391"/>
+            <a:gd name="connsiteX24" fmla="*/ 2500177 w 3614083"/>
+            <a:gd name="connsiteY24" fmla="*/ 2176786 h 2705391"/>
+            <a:gd name="connsiteX25" fmla="*/ 2915814 w 3614083"/>
+            <a:gd name="connsiteY25" fmla="*/ 1941259 h 2705391"/>
+            <a:gd name="connsiteX26" fmla="*/ 2583305 w 3614083"/>
+            <a:gd name="connsiteY26" fmla="*/ 722059 h 2705391"/>
+            <a:gd name="connsiteX27" fmla="*/ 1890577 w 3614083"/>
+            <a:gd name="connsiteY27" fmla="*/ 431114 h 2705391"/>
+            <a:gd name="connsiteX28" fmla="*/ 851487 w 3614083"/>
+            <a:gd name="connsiteY28" fmla="*/ 472677 h 2705391"/>
+            <a:gd name="connsiteX29" fmla="*/ 518977 w 3614083"/>
+            <a:gd name="connsiteY29" fmla="*/ 2065950 h 2705391"/>
+            <a:gd name="connsiteX30" fmla="*/ 1280977 w 3614083"/>
+            <a:gd name="connsiteY30" fmla="*/ 2481586 h 2705391"/>
+            <a:gd name="connsiteX31" fmla="*/ 2804977 w 3614083"/>
+            <a:gd name="connsiteY31" fmla="*/ 2329186 h 2705391"/>
+            <a:gd name="connsiteX32" fmla="*/ 3442287 w 3614083"/>
+            <a:gd name="connsiteY32" fmla="*/ 902168 h 2705391"/>
+            <a:gd name="connsiteX33" fmla="*/ 1959850 w 3614083"/>
+            <a:gd name="connsiteY33" fmla="*/ 361841 h 2705391"/>
+            <a:gd name="connsiteX34" fmla="*/ 1239414 w 3614083"/>
+            <a:gd name="connsiteY34" fmla="*/ 403404 h 2705391"/>
+            <a:gd name="connsiteX35" fmla="*/ 879196 w 3614083"/>
+            <a:gd name="connsiteY35" fmla="*/ 1622604 h 2705391"/>
+            <a:gd name="connsiteX36" fmla="*/ 1114723 w 3614083"/>
+            <a:gd name="connsiteY36" fmla="*/ 2315332 h 2705391"/>
+            <a:gd name="connsiteX37" fmla="*/ 3303741 w 3614083"/>
+            <a:gd name="connsiteY37" fmla="*/ 2329186 h 2705391"/>
+            <a:gd name="connsiteX38" fmla="*/ 3594687 w 3614083"/>
+            <a:gd name="connsiteY38" fmla="*/ 1788859 h 2705391"/>
+            <a:gd name="connsiteX39" fmla="*/ 2818832 w 3614083"/>
+            <a:gd name="connsiteY39" fmla="*/ 569659 h 2705391"/>
+            <a:gd name="connsiteX40" fmla="*/ 1807450 w 3614083"/>
+            <a:gd name="connsiteY40" fmla="*/ 389550 h 2705391"/>
+            <a:gd name="connsiteX41" fmla="*/ 712941 w 3614083"/>
+            <a:gd name="connsiteY41" fmla="*/ 555804 h 2705391"/>
+            <a:gd name="connsiteX42" fmla="*/ 809923 w 3614083"/>
+            <a:gd name="connsiteY42" fmla="*/ 1054568 h 2705391"/>
+            <a:gd name="connsiteX43" fmla="*/ 1530359 w 3614083"/>
+            <a:gd name="connsiteY43" fmla="*/ 1747295 h 2705391"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX0" y="connsiteY0"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX1" y="connsiteY1"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX2" y="connsiteY2"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX3" y="connsiteY3"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX4" y="connsiteY4"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX5" y="connsiteY5"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX6" y="connsiteY6"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX7" y="connsiteY7"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX8" y="connsiteY8"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX9" y="connsiteY9"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX10" y="connsiteY10"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX11" y="connsiteY11"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX12" y="connsiteY12"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX13" y="connsiteY13"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX14" y="connsiteY14"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX15" y="connsiteY15"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX16" y="connsiteY16"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX17" y="connsiteY17"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX18" y="connsiteY18"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX19" y="connsiteY19"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX20" y="connsiteY20"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX21" y="connsiteY21"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX22" y="connsiteY22"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX23" y="connsiteY23"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX24" y="connsiteY24"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX25" y="connsiteY25"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX26" y="connsiteY26"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX27" y="connsiteY27"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX28" y="connsiteY28"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX29" y="connsiteY29"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX30" y="connsiteY30"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX31" y="connsiteY31"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX32" y="connsiteY32"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX33" y="connsiteY33"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX34" y="connsiteY34"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX35" y="connsiteY35"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX36" y="connsiteY36"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX37" y="connsiteY37"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX38" y="connsiteY38"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX39" y="connsiteY39"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX40" y="connsiteY40"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX41" y="connsiteY41"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX42" y="connsiteY42"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX43" y="connsiteY43"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="3614083" h="2705391">
+              <a:moveTo>
+                <a:pt x="3220614" y="417259"/>
+              </a:moveTo>
+              <a:cubicBezTo>
+                <a:pt x="3192905" y="398786"/>
+                <a:pt x="3168281" y="374521"/>
+                <a:pt x="3137487" y="361841"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2639488" y="156782"/>
+                <a:pt x="2766428" y="223678"/>
+                <a:pt x="2139959" y="209441"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1993317" y="541829"/>
+                <a:pt x="1681159" y="1222173"/>
+                <a:pt x="1627341" y="1511768"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1512928" y="2127422"/>
+                <a:pt x="1571809" y="2462777"/>
+                <a:pt x="2236941" y="2661695"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2520251" y="2746423"/>
+                <a:pt x="2828068" y="2680168"/>
+                <a:pt x="3123632" y="2689404"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="3625280" y="2482844"/>
+                <a:pt x="3429978" y="2647086"/>
+                <a:pt x="3386868" y="1664168"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="3359010" y="1029008"/>
+                <a:pt x="3312696" y="768300"/>
+                <a:pt x="2638723" y="458823"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2423656" y="360068"/>
+                <a:pt x="2167668" y="412641"/>
+                <a:pt x="1932141" y="389550"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1839777" y="505005"/>
+                <a:pt x="1697307" y="594227"/>
+                <a:pt x="1655050" y="735914"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1579878" y="987961"/>
+                <a:pt x="1700423" y="1290674"/>
+                <a:pt x="1904432" y="1442495"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2018804" y="1527609"/>
+                <a:pt x="2152761" y="1593663"/>
+                <a:pt x="2292359" y="1622604"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2537218" y="1673367"/>
+                <a:pt x="2791123" y="1659550"/>
+                <a:pt x="3040505" y="1678023"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="3461274" y="1312136"/>
+                <a:pt x="3941912" y="1052970"/>
+                <a:pt x="3165196" y="223295"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2929918" y="-28025"/>
+                <a:pt x="2481705" y="140168"/>
+                <a:pt x="2139959" y="98604"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1691995" y="241768"/>
+                <a:pt x="1211844" y="308328"/>
+                <a:pt x="796068" y="528095"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="547781" y="659332"/>
+                <a:pt x="177703" y="843916"/>
+                <a:pt x="200323" y="1123841"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="257492" y="1831304"/>
+                <a:pt x="1754902" y="2250591"/>
+                <a:pt x="2112250" y="2398459"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2370868" y="2393841"/>
+                <a:pt x="2644246" y="2470847"/>
+                <a:pt x="2888105" y="2384604"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="3363385" y="2216517"/>
+                <a:pt x="3289941" y="1642924"/>
+                <a:pt x="3331450" y="1290095"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="3280650" y="980677"/>
+                <a:pt x="3371003" y="609781"/>
+                <a:pt x="3179050" y="361841"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2633079" y="-343371"/>
+                <a:pt x="1201273" y="185557"/>
+                <a:pt x="712941" y="264859"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="495886" y="472677"/>
+                <a:pt x="184364" y="613953"/>
+                <a:pt x="61777" y="888314"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="-31015" y="1095992"/>
+                <a:pt x="-28016" y="1404586"/>
+                <a:pt x="131050" y="1567186"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="880339" y="2333125"/>
+                <a:pt x="1575542" y="2166035"/>
+                <a:pt x="2500177" y="2176786"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2638723" y="2098277"/>
+                <a:pt x="2863411" y="2091633"/>
+                <a:pt x="2915814" y="1941259"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2976840" y="1766141"/>
+                <a:pt x="2750479" y="871767"/>
+                <a:pt x="2583305" y="722059"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2396733" y="554980"/>
+                <a:pt x="2121486" y="528096"/>
+                <a:pt x="1890577" y="431114"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1544214" y="444968"/>
+                <a:pt x="1149210" y="295136"/>
+                <a:pt x="851487" y="472677"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="434176" y="721532"/>
+                <a:pt x="187540" y="1642730"/>
+                <a:pt x="518977" y="2065950"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="697366" y="2293740"/>
+                <a:pt x="1026977" y="2343041"/>
+                <a:pt x="1280977" y="2481586"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1788977" y="2430786"/>
+                <a:pt x="2329100" y="2514081"/>
+                <a:pt x="2804977" y="2329186"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="3333571" y="2123809"/>
+                <a:pt x="3686325" y="1439053"/>
+                <a:pt x="3442287" y="902168"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="3253561" y="486970"/>
+                <a:pt x="2150412" y="400998"/>
+                <a:pt x="1959850" y="361841"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1719705" y="375695"/>
+                <a:pt x="1455121" y="296951"/>
+                <a:pt x="1239414" y="403404"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="759195" y="640395"/>
+                <a:pt x="886400" y="1240770"/>
+                <a:pt x="879196" y="1622604"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="957705" y="1853513"/>
+                <a:pt x="914552" y="2175997"/>
+                <a:pt x="1114723" y="2315332"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1929521" y="2882496"/>
+                <a:pt x="2509408" y="2546811"/>
+                <a:pt x="3303741" y="2329186"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="3400723" y="2149077"/>
+                <a:pt x="3563245" y="1990988"/>
+                <a:pt x="3594687" y="1788859"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="3694202" y="1149121"/>
+                <a:pt x="3407067" y="810739"/>
+                <a:pt x="2818832" y="569659"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2501979" y="439801"/>
+                <a:pt x="2144577" y="449586"/>
+                <a:pt x="1807450" y="389550"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1442614" y="444968"/>
+                <a:pt x="1019985" y="351108"/>
+                <a:pt x="712941" y="555804"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="572018" y="649753"/>
+                <a:pt x="723062" y="909169"/>
+                <a:pt x="809923" y="1054568"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1025925" y="1416137"/>
+                <a:pt x="1240076" y="1546330"/>
+                <a:pt x="1530359" y="1747295"/>
+              </a:cubicBezTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-PH" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>381568</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>53796</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>338051</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>57550</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Freeform: Shape 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F0C1316-2466-226E-DA89-019972DF3D4F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11354368" y="7659941"/>
+          <a:ext cx="3614083" cy="2705391"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="connsiteX0" fmla="*/ 3220614 w 3614083"/>
+            <a:gd name="connsiteY0" fmla="*/ 417259 h 2705391"/>
+            <a:gd name="connsiteX1" fmla="*/ 3137487 w 3614083"/>
+            <a:gd name="connsiteY1" fmla="*/ 361841 h 2705391"/>
+            <a:gd name="connsiteX2" fmla="*/ 2139959 w 3614083"/>
+            <a:gd name="connsiteY2" fmla="*/ 209441 h 2705391"/>
+            <a:gd name="connsiteX3" fmla="*/ 1627341 w 3614083"/>
+            <a:gd name="connsiteY3" fmla="*/ 1511768 h 2705391"/>
+            <a:gd name="connsiteX4" fmla="*/ 2236941 w 3614083"/>
+            <a:gd name="connsiteY4" fmla="*/ 2661695 h 2705391"/>
+            <a:gd name="connsiteX5" fmla="*/ 3123632 w 3614083"/>
+            <a:gd name="connsiteY5" fmla="*/ 2689404 h 2705391"/>
+            <a:gd name="connsiteX6" fmla="*/ 3386868 w 3614083"/>
+            <a:gd name="connsiteY6" fmla="*/ 1664168 h 2705391"/>
+            <a:gd name="connsiteX7" fmla="*/ 2638723 w 3614083"/>
+            <a:gd name="connsiteY7" fmla="*/ 458823 h 2705391"/>
+            <a:gd name="connsiteX8" fmla="*/ 1932141 w 3614083"/>
+            <a:gd name="connsiteY8" fmla="*/ 389550 h 2705391"/>
+            <a:gd name="connsiteX9" fmla="*/ 1655050 w 3614083"/>
+            <a:gd name="connsiteY9" fmla="*/ 735914 h 2705391"/>
+            <a:gd name="connsiteX10" fmla="*/ 1904432 w 3614083"/>
+            <a:gd name="connsiteY10" fmla="*/ 1442495 h 2705391"/>
+            <a:gd name="connsiteX11" fmla="*/ 2292359 w 3614083"/>
+            <a:gd name="connsiteY11" fmla="*/ 1622604 h 2705391"/>
+            <a:gd name="connsiteX12" fmla="*/ 3040505 w 3614083"/>
+            <a:gd name="connsiteY12" fmla="*/ 1678023 h 2705391"/>
+            <a:gd name="connsiteX13" fmla="*/ 3165196 w 3614083"/>
+            <a:gd name="connsiteY13" fmla="*/ 223295 h 2705391"/>
+            <a:gd name="connsiteX14" fmla="*/ 2139959 w 3614083"/>
+            <a:gd name="connsiteY14" fmla="*/ 98604 h 2705391"/>
+            <a:gd name="connsiteX15" fmla="*/ 796068 w 3614083"/>
+            <a:gd name="connsiteY15" fmla="*/ 528095 h 2705391"/>
+            <a:gd name="connsiteX16" fmla="*/ 200323 w 3614083"/>
+            <a:gd name="connsiteY16" fmla="*/ 1123841 h 2705391"/>
+            <a:gd name="connsiteX17" fmla="*/ 2112250 w 3614083"/>
+            <a:gd name="connsiteY17" fmla="*/ 2398459 h 2705391"/>
+            <a:gd name="connsiteX18" fmla="*/ 2888105 w 3614083"/>
+            <a:gd name="connsiteY18" fmla="*/ 2384604 h 2705391"/>
+            <a:gd name="connsiteX19" fmla="*/ 3331450 w 3614083"/>
+            <a:gd name="connsiteY19" fmla="*/ 1290095 h 2705391"/>
+            <a:gd name="connsiteX20" fmla="*/ 3179050 w 3614083"/>
+            <a:gd name="connsiteY20" fmla="*/ 361841 h 2705391"/>
+            <a:gd name="connsiteX21" fmla="*/ 712941 w 3614083"/>
+            <a:gd name="connsiteY21" fmla="*/ 264859 h 2705391"/>
+            <a:gd name="connsiteX22" fmla="*/ 61777 w 3614083"/>
+            <a:gd name="connsiteY22" fmla="*/ 888314 h 2705391"/>
+            <a:gd name="connsiteX23" fmla="*/ 131050 w 3614083"/>
+            <a:gd name="connsiteY23" fmla="*/ 1567186 h 2705391"/>
+            <a:gd name="connsiteX24" fmla="*/ 2500177 w 3614083"/>
+            <a:gd name="connsiteY24" fmla="*/ 2176786 h 2705391"/>
+            <a:gd name="connsiteX25" fmla="*/ 2915814 w 3614083"/>
+            <a:gd name="connsiteY25" fmla="*/ 1941259 h 2705391"/>
+            <a:gd name="connsiteX26" fmla="*/ 2583305 w 3614083"/>
+            <a:gd name="connsiteY26" fmla="*/ 722059 h 2705391"/>
+            <a:gd name="connsiteX27" fmla="*/ 1890577 w 3614083"/>
+            <a:gd name="connsiteY27" fmla="*/ 431114 h 2705391"/>
+            <a:gd name="connsiteX28" fmla="*/ 851487 w 3614083"/>
+            <a:gd name="connsiteY28" fmla="*/ 472677 h 2705391"/>
+            <a:gd name="connsiteX29" fmla="*/ 518977 w 3614083"/>
+            <a:gd name="connsiteY29" fmla="*/ 2065950 h 2705391"/>
+            <a:gd name="connsiteX30" fmla="*/ 1280977 w 3614083"/>
+            <a:gd name="connsiteY30" fmla="*/ 2481586 h 2705391"/>
+            <a:gd name="connsiteX31" fmla="*/ 2804977 w 3614083"/>
+            <a:gd name="connsiteY31" fmla="*/ 2329186 h 2705391"/>
+            <a:gd name="connsiteX32" fmla="*/ 3442287 w 3614083"/>
+            <a:gd name="connsiteY32" fmla="*/ 902168 h 2705391"/>
+            <a:gd name="connsiteX33" fmla="*/ 1959850 w 3614083"/>
+            <a:gd name="connsiteY33" fmla="*/ 361841 h 2705391"/>
+            <a:gd name="connsiteX34" fmla="*/ 1239414 w 3614083"/>
+            <a:gd name="connsiteY34" fmla="*/ 403404 h 2705391"/>
+            <a:gd name="connsiteX35" fmla="*/ 879196 w 3614083"/>
+            <a:gd name="connsiteY35" fmla="*/ 1622604 h 2705391"/>
+            <a:gd name="connsiteX36" fmla="*/ 1114723 w 3614083"/>
+            <a:gd name="connsiteY36" fmla="*/ 2315332 h 2705391"/>
+            <a:gd name="connsiteX37" fmla="*/ 3303741 w 3614083"/>
+            <a:gd name="connsiteY37" fmla="*/ 2329186 h 2705391"/>
+            <a:gd name="connsiteX38" fmla="*/ 3594687 w 3614083"/>
+            <a:gd name="connsiteY38" fmla="*/ 1788859 h 2705391"/>
+            <a:gd name="connsiteX39" fmla="*/ 2818832 w 3614083"/>
+            <a:gd name="connsiteY39" fmla="*/ 569659 h 2705391"/>
+            <a:gd name="connsiteX40" fmla="*/ 1807450 w 3614083"/>
+            <a:gd name="connsiteY40" fmla="*/ 389550 h 2705391"/>
+            <a:gd name="connsiteX41" fmla="*/ 712941 w 3614083"/>
+            <a:gd name="connsiteY41" fmla="*/ 555804 h 2705391"/>
+            <a:gd name="connsiteX42" fmla="*/ 809923 w 3614083"/>
+            <a:gd name="connsiteY42" fmla="*/ 1054568 h 2705391"/>
+            <a:gd name="connsiteX43" fmla="*/ 1530359 w 3614083"/>
+            <a:gd name="connsiteY43" fmla="*/ 1747295 h 2705391"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX0" y="connsiteY0"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX1" y="connsiteY1"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX2" y="connsiteY2"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX3" y="connsiteY3"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX4" y="connsiteY4"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX5" y="connsiteY5"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX6" y="connsiteY6"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX7" y="connsiteY7"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX8" y="connsiteY8"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX9" y="connsiteY9"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX10" y="connsiteY10"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX11" y="connsiteY11"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX12" y="connsiteY12"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX13" y="connsiteY13"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX14" y="connsiteY14"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX15" y="connsiteY15"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX16" y="connsiteY16"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX17" y="connsiteY17"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX18" y="connsiteY18"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX19" y="connsiteY19"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX20" y="connsiteY20"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX21" y="connsiteY21"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX22" y="connsiteY22"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX23" y="connsiteY23"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX24" y="connsiteY24"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX25" y="connsiteY25"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX26" y="connsiteY26"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX27" y="connsiteY27"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX28" y="connsiteY28"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX29" y="connsiteY29"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX30" y="connsiteY30"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX31" y="connsiteY31"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX32" y="connsiteY32"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX33" y="connsiteY33"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX34" y="connsiteY34"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX35" y="connsiteY35"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX36" y="connsiteY36"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX37" y="connsiteY37"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX38" y="connsiteY38"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX39" y="connsiteY39"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX40" y="connsiteY40"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX41" y="connsiteY41"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX42" y="connsiteY42"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX43" y="connsiteY43"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="3614083" h="2705391">
+              <a:moveTo>
+                <a:pt x="3220614" y="417259"/>
+              </a:moveTo>
+              <a:cubicBezTo>
+                <a:pt x="3192905" y="398786"/>
+                <a:pt x="3168281" y="374521"/>
+                <a:pt x="3137487" y="361841"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2639488" y="156782"/>
+                <a:pt x="2766428" y="223678"/>
+                <a:pt x="2139959" y="209441"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1993317" y="541829"/>
+                <a:pt x="1681159" y="1222173"/>
+                <a:pt x="1627341" y="1511768"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1512928" y="2127422"/>
+                <a:pt x="1571809" y="2462777"/>
+                <a:pt x="2236941" y="2661695"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2520251" y="2746423"/>
+                <a:pt x="2828068" y="2680168"/>
+                <a:pt x="3123632" y="2689404"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="3625280" y="2482844"/>
+                <a:pt x="3429978" y="2647086"/>
+                <a:pt x="3386868" y="1664168"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="3359010" y="1029008"/>
+                <a:pt x="3312696" y="768300"/>
+                <a:pt x="2638723" y="458823"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2423656" y="360068"/>
+                <a:pt x="2167668" y="412641"/>
+                <a:pt x="1932141" y="389550"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1839777" y="505005"/>
+                <a:pt x="1697307" y="594227"/>
+                <a:pt x="1655050" y="735914"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1579878" y="987961"/>
+                <a:pt x="1700423" y="1290674"/>
+                <a:pt x="1904432" y="1442495"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2018804" y="1527609"/>
+                <a:pt x="2152761" y="1593663"/>
+                <a:pt x="2292359" y="1622604"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2537218" y="1673367"/>
+                <a:pt x="2791123" y="1659550"/>
+                <a:pt x="3040505" y="1678023"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="3461274" y="1312136"/>
+                <a:pt x="3941912" y="1052970"/>
+                <a:pt x="3165196" y="223295"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2929918" y="-28025"/>
+                <a:pt x="2481705" y="140168"/>
+                <a:pt x="2139959" y="98604"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1691995" y="241768"/>
+                <a:pt x="1211844" y="308328"/>
+                <a:pt x="796068" y="528095"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="547781" y="659332"/>
+                <a:pt x="177703" y="843916"/>
+                <a:pt x="200323" y="1123841"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="257492" y="1831304"/>
+                <a:pt x="1754902" y="2250591"/>
+                <a:pt x="2112250" y="2398459"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2370868" y="2393841"/>
+                <a:pt x="2644246" y="2470847"/>
+                <a:pt x="2888105" y="2384604"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="3363385" y="2216517"/>
+                <a:pt x="3289941" y="1642924"/>
+                <a:pt x="3331450" y="1290095"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="3280650" y="980677"/>
+                <a:pt x="3371003" y="609781"/>
+                <a:pt x="3179050" y="361841"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2633079" y="-343371"/>
+                <a:pt x="1201273" y="185557"/>
+                <a:pt x="712941" y="264859"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="495886" y="472677"/>
+                <a:pt x="184364" y="613953"/>
+                <a:pt x="61777" y="888314"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="-31015" y="1095992"/>
+                <a:pt x="-28016" y="1404586"/>
+                <a:pt x="131050" y="1567186"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="880339" y="2333125"/>
+                <a:pt x="1575542" y="2166035"/>
+                <a:pt x="2500177" y="2176786"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2638723" y="2098277"/>
+                <a:pt x="2863411" y="2091633"/>
+                <a:pt x="2915814" y="1941259"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2976840" y="1766141"/>
+                <a:pt x="2750479" y="871767"/>
+                <a:pt x="2583305" y="722059"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2396733" y="554980"/>
+                <a:pt x="2121486" y="528096"/>
+                <a:pt x="1890577" y="431114"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1544214" y="444968"/>
+                <a:pt x="1149210" y="295136"/>
+                <a:pt x="851487" y="472677"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="434176" y="721532"/>
+                <a:pt x="187540" y="1642730"/>
+                <a:pt x="518977" y="2065950"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="697366" y="2293740"/>
+                <a:pt x="1026977" y="2343041"/>
+                <a:pt x="1280977" y="2481586"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1788977" y="2430786"/>
+                <a:pt x="2329100" y="2514081"/>
+                <a:pt x="2804977" y="2329186"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="3333571" y="2123809"/>
+                <a:pt x="3686325" y="1439053"/>
+                <a:pt x="3442287" y="902168"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="3253561" y="486970"/>
+                <a:pt x="2150412" y="400998"/>
+                <a:pt x="1959850" y="361841"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1719705" y="375695"/>
+                <a:pt x="1455121" y="296951"/>
+                <a:pt x="1239414" y="403404"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="759195" y="640395"/>
+                <a:pt x="886400" y="1240770"/>
+                <a:pt x="879196" y="1622604"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="957705" y="1853513"/>
+                <a:pt x="914552" y="2175997"/>
+                <a:pt x="1114723" y="2315332"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1929521" y="2882496"/>
+                <a:pt x="2509408" y="2546811"/>
+                <a:pt x="3303741" y="2329186"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="3400723" y="2149077"/>
+                <a:pt x="3563245" y="1990988"/>
+                <a:pt x="3594687" y="1788859"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="3694202" y="1149121"/>
+                <a:pt x="3407067" y="810739"/>
+                <a:pt x="2818832" y="569659"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2501979" y="439801"/>
+                <a:pt x="2144577" y="449586"/>
+                <a:pt x="1807450" y="389550"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1442614" y="444968"/>
+                <a:pt x="1019985" y="351108"/>
+                <a:pt x="712941" y="555804"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="572018" y="649753"/>
+                <a:pt x="723062" y="909169"/>
+                <a:pt x="809923" y="1054568"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1025925" y="1416137"/>
+                <a:pt x="1240076" y="1546330"/>
+                <a:pt x="1530359" y="1747295"/>
+              </a:cubicBezTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-PH" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>561677</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>150776</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>518160</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>154531</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Freeform: Shape 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AC0C4F0C-03E3-BC8E-50A2-23EB1E24F524}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2390477" y="7937031"/>
+          <a:ext cx="3614083" cy="2705391"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="connsiteX0" fmla="*/ 3220614 w 3614083"/>
+            <a:gd name="connsiteY0" fmla="*/ 417259 h 2705391"/>
+            <a:gd name="connsiteX1" fmla="*/ 3137487 w 3614083"/>
+            <a:gd name="connsiteY1" fmla="*/ 361841 h 2705391"/>
+            <a:gd name="connsiteX2" fmla="*/ 2139959 w 3614083"/>
+            <a:gd name="connsiteY2" fmla="*/ 209441 h 2705391"/>
+            <a:gd name="connsiteX3" fmla="*/ 1627341 w 3614083"/>
+            <a:gd name="connsiteY3" fmla="*/ 1511768 h 2705391"/>
+            <a:gd name="connsiteX4" fmla="*/ 2236941 w 3614083"/>
+            <a:gd name="connsiteY4" fmla="*/ 2661695 h 2705391"/>
+            <a:gd name="connsiteX5" fmla="*/ 3123632 w 3614083"/>
+            <a:gd name="connsiteY5" fmla="*/ 2689404 h 2705391"/>
+            <a:gd name="connsiteX6" fmla="*/ 3386868 w 3614083"/>
+            <a:gd name="connsiteY6" fmla="*/ 1664168 h 2705391"/>
+            <a:gd name="connsiteX7" fmla="*/ 2638723 w 3614083"/>
+            <a:gd name="connsiteY7" fmla="*/ 458823 h 2705391"/>
+            <a:gd name="connsiteX8" fmla="*/ 1932141 w 3614083"/>
+            <a:gd name="connsiteY8" fmla="*/ 389550 h 2705391"/>
+            <a:gd name="connsiteX9" fmla="*/ 1655050 w 3614083"/>
+            <a:gd name="connsiteY9" fmla="*/ 735914 h 2705391"/>
+            <a:gd name="connsiteX10" fmla="*/ 1904432 w 3614083"/>
+            <a:gd name="connsiteY10" fmla="*/ 1442495 h 2705391"/>
+            <a:gd name="connsiteX11" fmla="*/ 2292359 w 3614083"/>
+            <a:gd name="connsiteY11" fmla="*/ 1622604 h 2705391"/>
+            <a:gd name="connsiteX12" fmla="*/ 3040505 w 3614083"/>
+            <a:gd name="connsiteY12" fmla="*/ 1678023 h 2705391"/>
+            <a:gd name="connsiteX13" fmla="*/ 3165196 w 3614083"/>
+            <a:gd name="connsiteY13" fmla="*/ 223295 h 2705391"/>
+            <a:gd name="connsiteX14" fmla="*/ 2139959 w 3614083"/>
+            <a:gd name="connsiteY14" fmla="*/ 98604 h 2705391"/>
+            <a:gd name="connsiteX15" fmla="*/ 796068 w 3614083"/>
+            <a:gd name="connsiteY15" fmla="*/ 528095 h 2705391"/>
+            <a:gd name="connsiteX16" fmla="*/ 200323 w 3614083"/>
+            <a:gd name="connsiteY16" fmla="*/ 1123841 h 2705391"/>
+            <a:gd name="connsiteX17" fmla="*/ 2112250 w 3614083"/>
+            <a:gd name="connsiteY17" fmla="*/ 2398459 h 2705391"/>
+            <a:gd name="connsiteX18" fmla="*/ 2888105 w 3614083"/>
+            <a:gd name="connsiteY18" fmla="*/ 2384604 h 2705391"/>
+            <a:gd name="connsiteX19" fmla="*/ 3331450 w 3614083"/>
+            <a:gd name="connsiteY19" fmla="*/ 1290095 h 2705391"/>
+            <a:gd name="connsiteX20" fmla="*/ 3179050 w 3614083"/>
+            <a:gd name="connsiteY20" fmla="*/ 361841 h 2705391"/>
+            <a:gd name="connsiteX21" fmla="*/ 712941 w 3614083"/>
+            <a:gd name="connsiteY21" fmla="*/ 264859 h 2705391"/>
+            <a:gd name="connsiteX22" fmla="*/ 61777 w 3614083"/>
+            <a:gd name="connsiteY22" fmla="*/ 888314 h 2705391"/>
+            <a:gd name="connsiteX23" fmla="*/ 131050 w 3614083"/>
+            <a:gd name="connsiteY23" fmla="*/ 1567186 h 2705391"/>
+            <a:gd name="connsiteX24" fmla="*/ 2500177 w 3614083"/>
+            <a:gd name="connsiteY24" fmla="*/ 2176786 h 2705391"/>
+            <a:gd name="connsiteX25" fmla="*/ 2915814 w 3614083"/>
+            <a:gd name="connsiteY25" fmla="*/ 1941259 h 2705391"/>
+            <a:gd name="connsiteX26" fmla="*/ 2583305 w 3614083"/>
+            <a:gd name="connsiteY26" fmla="*/ 722059 h 2705391"/>
+            <a:gd name="connsiteX27" fmla="*/ 1890577 w 3614083"/>
+            <a:gd name="connsiteY27" fmla="*/ 431114 h 2705391"/>
+            <a:gd name="connsiteX28" fmla="*/ 851487 w 3614083"/>
+            <a:gd name="connsiteY28" fmla="*/ 472677 h 2705391"/>
+            <a:gd name="connsiteX29" fmla="*/ 518977 w 3614083"/>
+            <a:gd name="connsiteY29" fmla="*/ 2065950 h 2705391"/>
+            <a:gd name="connsiteX30" fmla="*/ 1280977 w 3614083"/>
+            <a:gd name="connsiteY30" fmla="*/ 2481586 h 2705391"/>
+            <a:gd name="connsiteX31" fmla="*/ 2804977 w 3614083"/>
+            <a:gd name="connsiteY31" fmla="*/ 2329186 h 2705391"/>
+            <a:gd name="connsiteX32" fmla="*/ 3442287 w 3614083"/>
+            <a:gd name="connsiteY32" fmla="*/ 902168 h 2705391"/>
+            <a:gd name="connsiteX33" fmla="*/ 1959850 w 3614083"/>
+            <a:gd name="connsiteY33" fmla="*/ 361841 h 2705391"/>
+            <a:gd name="connsiteX34" fmla="*/ 1239414 w 3614083"/>
+            <a:gd name="connsiteY34" fmla="*/ 403404 h 2705391"/>
+            <a:gd name="connsiteX35" fmla="*/ 879196 w 3614083"/>
+            <a:gd name="connsiteY35" fmla="*/ 1622604 h 2705391"/>
+            <a:gd name="connsiteX36" fmla="*/ 1114723 w 3614083"/>
+            <a:gd name="connsiteY36" fmla="*/ 2315332 h 2705391"/>
+            <a:gd name="connsiteX37" fmla="*/ 3303741 w 3614083"/>
+            <a:gd name="connsiteY37" fmla="*/ 2329186 h 2705391"/>
+            <a:gd name="connsiteX38" fmla="*/ 3594687 w 3614083"/>
+            <a:gd name="connsiteY38" fmla="*/ 1788859 h 2705391"/>
+            <a:gd name="connsiteX39" fmla="*/ 2818832 w 3614083"/>
+            <a:gd name="connsiteY39" fmla="*/ 569659 h 2705391"/>
+            <a:gd name="connsiteX40" fmla="*/ 1807450 w 3614083"/>
+            <a:gd name="connsiteY40" fmla="*/ 389550 h 2705391"/>
+            <a:gd name="connsiteX41" fmla="*/ 712941 w 3614083"/>
+            <a:gd name="connsiteY41" fmla="*/ 555804 h 2705391"/>
+            <a:gd name="connsiteX42" fmla="*/ 809923 w 3614083"/>
+            <a:gd name="connsiteY42" fmla="*/ 1054568 h 2705391"/>
+            <a:gd name="connsiteX43" fmla="*/ 1530359 w 3614083"/>
+            <a:gd name="connsiteY43" fmla="*/ 1747295 h 2705391"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX0" y="connsiteY0"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX1" y="connsiteY1"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX2" y="connsiteY2"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX3" y="connsiteY3"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX4" y="connsiteY4"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX5" y="connsiteY5"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX6" y="connsiteY6"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX7" y="connsiteY7"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX8" y="connsiteY8"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX9" y="connsiteY9"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX10" y="connsiteY10"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX11" y="connsiteY11"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX12" y="connsiteY12"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX13" y="connsiteY13"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX14" y="connsiteY14"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX15" y="connsiteY15"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX16" y="connsiteY16"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX17" y="connsiteY17"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX18" y="connsiteY18"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX19" y="connsiteY19"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX20" y="connsiteY20"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX21" y="connsiteY21"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX22" y="connsiteY22"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX23" y="connsiteY23"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX24" y="connsiteY24"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX25" y="connsiteY25"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX26" y="connsiteY26"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX27" y="connsiteY27"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX28" y="connsiteY28"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX29" y="connsiteY29"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX30" y="connsiteY30"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX31" y="connsiteY31"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX32" y="connsiteY32"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX33" y="connsiteY33"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX34" y="connsiteY34"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX35" y="connsiteY35"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX36" y="connsiteY36"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX37" y="connsiteY37"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX38" y="connsiteY38"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX39" y="connsiteY39"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX40" y="connsiteY40"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX41" y="connsiteY41"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX42" y="connsiteY42"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX43" y="connsiteY43"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="3614083" h="2705391">
+              <a:moveTo>
+                <a:pt x="3220614" y="417259"/>
+              </a:moveTo>
+              <a:cubicBezTo>
+                <a:pt x="3192905" y="398786"/>
+                <a:pt x="3168281" y="374521"/>
+                <a:pt x="3137487" y="361841"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2639488" y="156782"/>
+                <a:pt x="2766428" y="223678"/>
+                <a:pt x="2139959" y="209441"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1993317" y="541829"/>
+                <a:pt x="1681159" y="1222173"/>
+                <a:pt x="1627341" y="1511768"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1512928" y="2127422"/>
+                <a:pt x="1571809" y="2462777"/>
+                <a:pt x="2236941" y="2661695"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2520251" y="2746423"/>
+                <a:pt x="2828068" y="2680168"/>
+                <a:pt x="3123632" y="2689404"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="3625280" y="2482844"/>
+                <a:pt x="3429978" y="2647086"/>
+                <a:pt x="3386868" y="1664168"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="3359010" y="1029008"/>
+                <a:pt x="3312696" y="768300"/>
+                <a:pt x="2638723" y="458823"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2423656" y="360068"/>
+                <a:pt x="2167668" y="412641"/>
+                <a:pt x="1932141" y="389550"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1839777" y="505005"/>
+                <a:pt x="1697307" y="594227"/>
+                <a:pt x="1655050" y="735914"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1579878" y="987961"/>
+                <a:pt x="1700423" y="1290674"/>
+                <a:pt x="1904432" y="1442495"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2018804" y="1527609"/>
+                <a:pt x="2152761" y="1593663"/>
+                <a:pt x="2292359" y="1622604"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2537218" y="1673367"/>
+                <a:pt x="2791123" y="1659550"/>
+                <a:pt x="3040505" y="1678023"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="3461274" y="1312136"/>
+                <a:pt x="3941912" y="1052970"/>
+                <a:pt x="3165196" y="223295"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2929918" y="-28025"/>
+                <a:pt x="2481705" y="140168"/>
+                <a:pt x="2139959" y="98604"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1691995" y="241768"/>
+                <a:pt x="1211844" y="308328"/>
+                <a:pt x="796068" y="528095"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="547781" y="659332"/>
+                <a:pt x="177703" y="843916"/>
+                <a:pt x="200323" y="1123841"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="257492" y="1831304"/>
+                <a:pt x="1754902" y="2250591"/>
+                <a:pt x="2112250" y="2398459"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2370868" y="2393841"/>
+                <a:pt x="2644246" y="2470847"/>
+                <a:pt x="2888105" y="2384604"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="3363385" y="2216517"/>
+                <a:pt x="3289941" y="1642924"/>
+                <a:pt x="3331450" y="1290095"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="3280650" y="980677"/>
+                <a:pt x="3371003" y="609781"/>
+                <a:pt x="3179050" y="361841"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2633079" y="-343371"/>
+                <a:pt x="1201273" y="185557"/>
+                <a:pt x="712941" y="264859"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="495886" y="472677"/>
+                <a:pt x="184364" y="613953"/>
+                <a:pt x="61777" y="888314"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="-31015" y="1095992"/>
+                <a:pt x="-28016" y="1404586"/>
+                <a:pt x="131050" y="1567186"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="880339" y="2333125"/>
+                <a:pt x="1575542" y="2166035"/>
+                <a:pt x="2500177" y="2176786"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2638723" y="2098277"/>
+                <a:pt x="2863411" y="2091633"/>
+                <a:pt x="2915814" y="1941259"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2976840" y="1766141"/>
+                <a:pt x="2750479" y="871767"/>
+                <a:pt x="2583305" y="722059"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2396733" y="554980"/>
+                <a:pt x="2121486" y="528096"/>
+                <a:pt x="1890577" y="431114"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1544214" y="444968"/>
+                <a:pt x="1149210" y="295136"/>
+                <a:pt x="851487" y="472677"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="434176" y="721532"/>
+                <a:pt x="187540" y="1642730"/>
+                <a:pt x="518977" y="2065950"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="697366" y="2293740"/>
+                <a:pt x="1026977" y="2343041"/>
+                <a:pt x="1280977" y="2481586"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1788977" y="2430786"/>
+                <a:pt x="2329100" y="2514081"/>
+                <a:pt x="2804977" y="2329186"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="3333571" y="2123809"/>
+                <a:pt x="3686325" y="1439053"/>
+                <a:pt x="3442287" y="902168"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="3253561" y="486970"/>
+                <a:pt x="2150412" y="400998"/>
+                <a:pt x="1959850" y="361841"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1719705" y="375695"/>
+                <a:pt x="1455121" y="296951"/>
+                <a:pt x="1239414" y="403404"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="759195" y="640395"/>
+                <a:pt x="886400" y="1240770"/>
+                <a:pt x="879196" y="1622604"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="957705" y="1853513"/>
+                <a:pt x="914552" y="2175997"/>
+                <a:pt x="1114723" y="2315332"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1929521" y="2882496"/>
+                <a:pt x="2509408" y="2546811"/>
+                <a:pt x="3303741" y="2329186"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="3400723" y="2149077"/>
+                <a:pt x="3563245" y="1990988"/>
+                <a:pt x="3594687" y="1788859"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="3694202" y="1149121"/>
+                <a:pt x="3407067" y="810739"/>
+                <a:pt x="2818832" y="569659"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2501979" y="439801"/>
+                <a:pt x="2144577" y="449586"/>
+                <a:pt x="1807450" y="389550"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1442614" y="444968"/>
+                <a:pt x="1019985" y="351108"/>
+                <a:pt x="712941" y="555804"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="572018" y="649753"/>
+                <a:pt x="723062" y="909169"/>
+                <a:pt x="809923" y="1054568"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1025925" y="1416137"/>
+                <a:pt x="1240076" y="1546330"/>
+                <a:pt x="1530359" y="1747295"/>
+              </a:cubicBezTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-PH" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>512618</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>55418</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>554182</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>41563</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Freeform: Shape 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B48C404E-27E6-5AA6-B6D8-C5F63AD8C9C0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4779818" y="10002982"/>
+          <a:ext cx="3699164" cy="2327563"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="connsiteX0" fmla="*/ 0 w 3699164"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 2327563"/>
+            <a:gd name="connsiteX1" fmla="*/ 166255 w 3699164"/>
+            <a:gd name="connsiteY1" fmla="*/ 304800 h 2327563"/>
+            <a:gd name="connsiteX2" fmla="*/ 1260764 w 3699164"/>
+            <a:gd name="connsiteY2" fmla="*/ 1108363 h 2327563"/>
+            <a:gd name="connsiteX3" fmla="*/ 2424546 w 3699164"/>
+            <a:gd name="connsiteY3" fmla="*/ 1731818 h 2327563"/>
+            <a:gd name="connsiteX4" fmla="*/ 2549237 w 3699164"/>
+            <a:gd name="connsiteY4" fmla="*/ 1814945 h 2327563"/>
+            <a:gd name="connsiteX5" fmla="*/ 2951018 w 3699164"/>
+            <a:gd name="connsiteY5" fmla="*/ 2022763 h 2327563"/>
+            <a:gd name="connsiteX6" fmla="*/ 3366655 w 3699164"/>
+            <a:gd name="connsiteY6" fmla="*/ 2175163 h 2327563"/>
+            <a:gd name="connsiteX7" fmla="*/ 3699164 w 3699164"/>
+            <a:gd name="connsiteY7" fmla="*/ 2327563 h 2327563"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX0" y="connsiteY0"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX1" y="connsiteY1"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX2" y="connsiteY2"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX3" y="connsiteY3"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX4" y="connsiteY4"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX5" y="connsiteY5"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX6" y="connsiteY6"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX7" y="connsiteY7"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="3699164" h="2327563">
+              <a:moveTo>
+                <a:pt x="0" y="0"/>
+              </a:moveTo>
+              <a:cubicBezTo>
+                <a:pt x="21277" y="191487"/>
+                <a:pt x="-10783" y="114144"/>
+                <a:pt x="166255" y="304800"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="530272" y="696818"/>
+                <a:pt x="640189" y="703640"/>
+                <a:pt x="1260764" y="1108363"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1759545" y="1433655"/>
+                <a:pt x="1773909" y="1391485"/>
+                <a:pt x="2424546" y="1731818"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2468810" y="1754971"/>
+                <a:pt x="2505516" y="1790783"/>
+                <a:pt x="2549237" y="1814945"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2681207" y="1887876"/>
+                <a:pt x="2813040" y="1961959"/>
+                <a:pt x="2951018" y="2022763"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="3086053" y="2082270"/>
+                <a:pt x="3230441" y="2118407"/>
+                <a:pt x="3366655" y="2175163"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="3917670" y="2404752"/>
+                <a:pt x="3441283" y="2241603"/>
+                <a:pt x="3699164" y="2327563"/>
+              </a:cubicBezTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-PH" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>554182</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>27709</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>595746</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>13854</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="Freeform: Shape 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6634EA1C-FF12-089B-19A0-609B73543DDC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4211782" y="10155382"/>
+          <a:ext cx="3699164" cy="2327563"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="connsiteX0" fmla="*/ 0 w 3699164"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 2327563"/>
+            <a:gd name="connsiteX1" fmla="*/ 166255 w 3699164"/>
+            <a:gd name="connsiteY1" fmla="*/ 304800 h 2327563"/>
+            <a:gd name="connsiteX2" fmla="*/ 1260764 w 3699164"/>
+            <a:gd name="connsiteY2" fmla="*/ 1108363 h 2327563"/>
+            <a:gd name="connsiteX3" fmla="*/ 2424546 w 3699164"/>
+            <a:gd name="connsiteY3" fmla="*/ 1731818 h 2327563"/>
+            <a:gd name="connsiteX4" fmla="*/ 2549237 w 3699164"/>
+            <a:gd name="connsiteY4" fmla="*/ 1814945 h 2327563"/>
+            <a:gd name="connsiteX5" fmla="*/ 2951018 w 3699164"/>
+            <a:gd name="connsiteY5" fmla="*/ 2022763 h 2327563"/>
+            <a:gd name="connsiteX6" fmla="*/ 3366655 w 3699164"/>
+            <a:gd name="connsiteY6" fmla="*/ 2175163 h 2327563"/>
+            <a:gd name="connsiteX7" fmla="*/ 3699164 w 3699164"/>
+            <a:gd name="connsiteY7" fmla="*/ 2327563 h 2327563"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX0" y="connsiteY0"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX1" y="connsiteY1"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX2" y="connsiteY2"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX3" y="connsiteY3"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX4" y="connsiteY4"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX5" y="connsiteY5"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX6" y="connsiteY6"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX7" y="connsiteY7"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="3699164" h="2327563">
+              <a:moveTo>
+                <a:pt x="0" y="0"/>
+              </a:moveTo>
+              <a:cubicBezTo>
+                <a:pt x="21277" y="191487"/>
+                <a:pt x="-10783" y="114144"/>
+                <a:pt x="166255" y="304800"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="530272" y="696818"/>
+                <a:pt x="640189" y="703640"/>
+                <a:pt x="1260764" y="1108363"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1759545" y="1433655"/>
+                <a:pt x="1773909" y="1391485"/>
+                <a:pt x="2424546" y="1731818"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2468810" y="1754971"/>
+                <a:pt x="2505516" y="1790783"/>
+                <a:pt x="2549237" y="1814945"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2681207" y="1887876"/>
+                <a:pt x="2813040" y="1961959"/>
+                <a:pt x="2951018" y="2022763"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="3086053" y="2082270"/>
+                <a:pt x="3230441" y="2118407"/>
+                <a:pt x="3366655" y="2175163"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="3917670" y="2404752"/>
+                <a:pt x="3441283" y="2241603"/>
+                <a:pt x="3699164" y="2327563"/>
+              </a:cubicBezTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-PH" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>83127</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>27709</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>318655</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>83127</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="Freeform: Shape 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3438B005-D084-E622-6A2D-98F0BF7F7131}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11055927" y="9254836"/>
+          <a:ext cx="1454728" cy="2757055"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="connsiteX0" fmla="*/ 1454728 w 1454728"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 2757055"/>
+            <a:gd name="connsiteX1" fmla="*/ 1330037 w 1454728"/>
+            <a:gd name="connsiteY1" fmla="*/ 360219 h 2757055"/>
+            <a:gd name="connsiteX2" fmla="*/ 762000 w 1454728"/>
+            <a:gd name="connsiteY2" fmla="*/ 1149928 h 2757055"/>
+            <a:gd name="connsiteX3" fmla="*/ 554182 w 1454728"/>
+            <a:gd name="connsiteY3" fmla="*/ 1427019 h 2757055"/>
+            <a:gd name="connsiteX4" fmla="*/ 207818 w 1454728"/>
+            <a:gd name="connsiteY4" fmla="*/ 2189019 h 2757055"/>
+            <a:gd name="connsiteX5" fmla="*/ 166255 w 1454728"/>
+            <a:gd name="connsiteY5" fmla="*/ 2286000 h 2757055"/>
+            <a:gd name="connsiteX6" fmla="*/ 83128 w 1454728"/>
+            <a:gd name="connsiteY6" fmla="*/ 2466109 h 2757055"/>
+            <a:gd name="connsiteX7" fmla="*/ 0 w 1454728"/>
+            <a:gd name="connsiteY7" fmla="*/ 2757055 h 2757055"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX0" y="connsiteY0"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX1" y="connsiteY1"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX2" y="connsiteY2"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX3" y="connsiteY3"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX4" y="connsiteY4"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX5" y="connsiteY5"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX6" y="connsiteY6"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX7" y="connsiteY7"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="1454728" h="2757055">
+              <a:moveTo>
+                <a:pt x="1454728" y="0"/>
+              </a:moveTo>
+              <a:cubicBezTo>
+                <a:pt x="1413164" y="120073"/>
+                <a:pt x="1395603" y="251379"/>
+                <a:pt x="1330037" y="360219"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1162714" y="637975"/>
+                <a:pt x="952721" y="887687"/>
+                <a:pt x="762000" y="1149928"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="694093" y="1243300"/>
+                <a:pt x="612720" y="1327505"/>
+                <a:pt x="554182" y="1427019"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="315126" y="1833415"/>
+                <a:pt x="459132" y="1560736"/>
+                <a:pt x="207818" y="2189019"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="194756" y="2221674"/>
+                <a:pt x="180688" y="2253927"/>
+                <a:pt x="166255" y="2286000"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="139121" y="2346298"/>
+                <a:pt x="104038" y="2403380"/>
+                <a:pt x="83128" y="2466109"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="32746" y="2617251"/>
+                <a:pt x="62944" y="2521015"/>
+                <a:pt x="0" y="2757055"/>
+              </a:cubicBezTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-PH" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>526472</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>83127</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>138545</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="Freeform: Shape 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F57A538-F577-2959-C504-B426B58A232C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11499272" y="9490363"/>
+          <a:ext cx="1454728" cy="2757055"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="connsiteX0" fmla="*/ 1454728 w 1454728"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 2757055"/>
+            <a:gd name="connsiteX1" fmla="*/ 1330037 w 1454728"/>
+            <a:gd name="connsiteY1" fmla="*/ 360219 h 2757055"/>
+            <a:gd name="connsiteX2" fmla="*/ 762000 w 1454728"/>
+            <a:gd name="connsiteY2" fmla="*/ 1149928 h 2757055"/>
+            <a:gd name="connsiteX3" fmla="*/ 554182 w 1454728"/>
+            <a:gd name="connsiteY3" fmla="*/ 1427019 h 2757055"/>
+            <a:gd name="connsiteX4" fmla="*/ 207818 w 1454728"/>
+            <a:gd name="connsiteY4" fmla="*/ 2189019 h 2757055"/>
+            <a:gd name="connsiteX5" fmla="*/ 166255 w 1454728"/>
+            <a:gd name="connsiteY5" fmla="*/ 2286000 h 2757055"/>
+            <a:gd name="connsiteX6" fmla="*/ 83128 w 1454728"/>
+            <a:gd name="connsiteY6" fmla="*/ 2466109 h 2757055"/>
+            <a:gd name="connsiteX7" fmla="*/ 0 w 1454728"/>
+            <a:gd name="connsiteY7" fmla="*/ 2757055 h 2757055"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX0" y="connsiteY0"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX1" y="connsiteY1"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX2" y="connsiteY2"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX3" y="connsiteY3"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX4" y="connsiteY4"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX5" y="connsiteY5"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX6" y="connsiteY6"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX7" y="connsiteY7"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="1454728" h="2757055">
+              <a:moveTo>
+                <a:pt x="1454728" y="0"/>
+              </a:moveTo>
+              <a:cubicBezTo>
+                <a:pt x="1413164" y="120073"/>
+                <a:pt x="1395603" y="251379"/>
+                <a:pt x="1330037" y="360219"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1162714" y="637975"/>
+                <a:pt x="952721" y="887687"/>
+                <a:pt x="762000" y="1149928"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="694093" y="1243300"/>
+                <a:pt x="612720" y="1327505"/>
+                <a:pt x="554182" y="1427019"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="315126" y="1833415"/>
+                <a:pt x="459132" y="1560736"/>
+                <a:pt x="207818" y="2189019"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="194756" y="2221674"/>
+                <a:pt x="180688" y="2253927"/>
+                <a:pt x="166255" y="2286000"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="139121" y="2346298"/>
+                <a:pt x="104038" y="2403380"/>
+                <a:pt x="83128" y="2466109"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="32746" y="2617251"/>
+                <a:pt x="62944" y="2521015"/>
+                <a:pt x="0" y="2757055"/>
+              </a:cubicBezTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-PH" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>83127</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>83128</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>290147</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>138546</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="Freeform: Shape 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D57090D-07C9-CDD8-94EE-7B2C237FC1AC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9227127" y="3726873"/>
+          <a:ext cx="2645420" cy="9240982"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="connsiteX0" fmla="*/ 0 w 2645420"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 9240982"/>
+            <a:gd name="connsiteX1" fmla="*/ 997528 w 2645420"/>
+            <a:gd name="connsiteY1" fmla="*/ 180109 h 9240982"/>
+            <a:gd name="connsiteX2" fmla="*/ 1246909 w 2645420"/>
+            <a:gd name="connsiteY2" fmla="*/ 235527 h 9240982"/>
+            <a:gd name="connsiteX3" fmla="*/ 1953491 w 2645420"/>
+            <a:gd name="connsiteY3" fmla="*/ 651163 h 9240982"/>
+            <a:gd name="connsiteX4" fmla="*/ 2341418 w 2645420"/>
+            <a:gd name="connsiteY4" fmla="*/ 983672 h 9240982"/>
+            <a:gd name="connsiteX5" fmla="*/ 2452255 w 2645420"/>
+            <a:gd name="connsiteY5" fmla="*/ 1108363 h 9240982"/>
+            <a:gd name="connsiteX6" fmla="*/ 2549237 w 2645420"/>
+            <a:gd name="connsiteY6" fmla="*/ 1316182 h 9240982"/>
+            <a:gd name="connsiteX7" fmla="*/ 2604655 w 2645420"/>
+            <a:gd name="connsiteY7" fmla="*/ 1634836 h 9240982"/>
+            <a:gd name="connsiteX8" fmla="*/ 2618509 w 2645420"/>
+            <a:gd name="connsiteY8" fmla="*/ 3477491 h 9240982"/>
+            <a:gd name="connsiteX9" fmla="*/ 2563091 w 2645420"/>
+            <a:gd name="connsiteY9" fmla="*/ 3865418 h 9240982"/>
+            <a:gd name="connsiteX10" fmla="*/ 2410691 w 2645420"/>
+            <a:gd name="connsiteY10" fmla="*/ 4391891 h 9240982"/>
+            <a:gd name="connsiteX11" fmla="*/ 2022764 w 2645420"/>
+            <a:gd name="connsiteY11" fmla="*/ 5167745 h 9240982"/>
+            <a:gd name="connsiteX12" fmla="*/ 1759528 w 2645420"/>
+            <a:gd name="connsiteY12" fmla="*/ 5611091 h 9240982"/>
+            <a:gd name="connsiteX13" fmla="*/ 1704109 w 2645420"/>
+            <a:gd name="connsiteY13" fmla="*/ 5791200 h 9240982"/>
+            <a:gd name="connsiteX14" fmla="*/ 1468582 w 2645420"/>
+            <a:gd name="connsiteY14" fmla="*/ 6206836 h 9240982"/>
+            <a:gd name="connsiteX15" fmla="*/ 1371600 w 2645420"/>
+            <a:gd name="connsiteY15" fmla="*/ 6622472 h 9240982"/>
+            <a:gd name="connsiteX16" fmla="*/ 1316182 w 2645420"/>
+            <a:gd name="connsiteY16" fmla="*/ 6830291 h 9240982"/>
+            <a:gd name="connsiteX17" fmla="*/ 1260764 w 2645420"/>
+            <a:gd name="connsiteY17" fmla="*/ 7093527 h 9240982"/>
+            <a:gd name="connsiteX18" fmla="*/ 1108364 w 2645420"/>
+            <a:gd name="connsiteY18" fmla="*/ 7426036 h 9240982"/>
+            <a:gd name="connsiteX19" fmla="*/ 1025237 w 2645420"/>
+            <a:gd name="connsiteY19" fmla="*/ 7744691 h 9240982"/>
+            <a:gd name="connsiteX20" fmla="*/ 983673 w 2645420"/>
+            <a:gd name="connsiteY20" fmla="*/ 8174182 h 9240982"/>
+            <a:gd name="connsiteX21" fmla="*/ 845128 w 2645420"/>
+            <a:gd name="connsiteY21" fmla="*/ 8700654 h 9240982"/>
+            <a:gd name="connsiteX22" fmla="*/ 789709 w 2645420"/>
+            <a:gd name="connsiteY22" fmla="*/ 8991600 h 9240982"/>
+            <a:gd name="connsiteX23" fmla="*/ 775855 w 2645420"/>
+            <a:gd name="connsiteY23" fmla="*/ 9240982 h 9240982"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX0" y="connsiteY0"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX1" y="connsiteY1"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX2" y="connsiteY2"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX3" y="connsiteY3"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX4" y="connsiteY4"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX5" y="connsiteY5"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX6" y="connsiteY6"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX7" y="connsiteY7"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX8" y="connsiteY8"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX9" y="connsiteY9"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX10" y="connsiteY10"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX11" y="connsiteY11"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX12" y="connsiteY12"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX13" y="connsiteY13"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX14" y="connsiteY14"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX15" y="connsiteY15"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX16" y="connsiteY16"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX17" y="connsiteY17"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX18" y="connsiteY18"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX19" y="connsiteY19"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX20" y="connsiteY20"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX21" y="connsiteY21"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX22" y="connsiteY22"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX23" y="connsiteY23"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="2645420" h="9240982">
+              <a:moveTo>
+                <a:pt x="0" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="997528" y="180109"/>
+              </a:lnTo>
+              <a:cubicBezTo>
+                <a:pt x="1081203" y="195914"/>
+                <a:pt x="1167950" y="203640"/>
+                <a:pt x="1246909" y="235527"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1586222" y="372557"/>
+                <a:pt x="1702450" y="444751"/>
+                <a:pt x="1953491" y="651163"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2085043" y="759328"/>
+                <a:pt x="2215873" y="868589"/>
+                <a:pt x="2341418" y="983672"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2382411" y="1021249"/>
+                <a:pt x="2422782" y="1061205"/>
+                <a:pt x="2452255" y="1108363"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2492771" y="1173188"/>
+                <a:pt x="2516910" y="1246909"/>
+                <a:pt x="2549237" y="1316182"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2567710" y="1422400"/>
+                <a:pt x="2590406" y="1527969"/>
+                <a:pt x="2604655" y="1634836"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2679196" y="2193893"/>
+                <a:pt x="2631174" y="3125399"/>
+                <a:pt x="2618509" y="3477491"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2613813" y="3608028"/>
+                <a:pt x="2585954" y="3736813"/>
+                <a:pt x="2563091" y="3865418"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2535073" y="4023019"/>
+                <a:pt x="2468770" y="4249332"/>
+                <a:pt x="2410691" y="4391891"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2282719" y="4706005"/>
+                <a:pt x="2190254" y="4888596"/>
+                <a:pt x="2022764" y="5167745"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1956807" y="5277674"/>
+                <a:pt x="1815889" y="5467058"/>
+                <a:pt x="1759528" y="5611091"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1736639" y="5669586"/>
+                <a:pt x="1733771" y="5735831"/>
+                <a:pt x="1704109" y="5791200"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1478795" y="6211784"/>
+                <a:pt x="1608620" y="5786721"/>
+                <a:pt x="1468582" y="6206836"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1406548" y="6392939"/>
+                <a:pt x="1415808" y="6433011"/>
+                <a:pt x="1371600" y="6622472"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1355309" y="6692290"/>
+                <a:pt x="1332603" y="6760503"/>
+                <a:pt x="1316182" y="6830291"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1295644" y="6917576"/>
+                <a:pt x="1290298" y="7008862"/>
+                <a:pt x="1260764" y="7093527"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1220606" y="7208647"/>
+                <a:pt x="1139140" y="7308061"/>
+                <a:pt x="1108364" y="7426036"/>
+              </a:cubicBezTo>
+              <a:lnTo>
+                <a:pt x="1025237" y="7744691"/>
+              </a:lnTo>
+              <a:cubicBezTo>
+                <a:pt x="1011382" y="7887855"/>
+                <a:pt x="1029157" y="8037731"/>
+                <a:pt x="983673" y="8174182"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="914443" y="8381873"/>
+                <a:pt x="928367" y="8333016"/>
+                <a:pt x="845128" y="8700654"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="823327" y="8796942"/>
+                <a:pt x="802263" y="8893676"/>
+                <a:pt x="789709" y="8991600"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="779122" y="9074180"/>
+                <a:pt x="780473" y="9157855"/>
+                <a:pt x="775855" y="9240982"/>
+              </a:cubicBezTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-PH" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>443345</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>13855</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>40765</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>69273</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="Freeform: Shape 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59A4C563-50C0-DDF2-1CD9-D9CF44D39B5D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9587345" y="3657600"/>
+          <a:ext cx="2645420" cy="9240982"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="connsiteX0" fmla="*/ 0 w 2645420"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 9240982"/>
+            <a:gd name="connsiteX1" fmla="*/ 997528 w 2645420"/>
+            <a:gd name="connsiteY1" fmla="*/ 180109 h 9240982"/>
+            <a:gd name="connsiteX2" fmla="*/ 1246909 w 2645420"/>
+            <a:gd name="connsiteY2" fmla="*/ 235527 h 9240982"/>
+            <a:gd name="connsiteX3" fmla="*/ 1953491 w 2645420"/>
+            <a:gd name="connsiteY3" fmla="*/ 651163 h 9240982"/>
+            <a:gd name="connsiteX4" fmla="*/ 2341418 w 2645420"/>
+            <a:gd name="connsiteY4" fmla="*/ 983672 h 9240982"/>
+            <a:gd name="connsiteX5" fmla="*/ 2452255 w 2645420"/>
+            <a:gd name="connsiteY5" fmla="*/ 1108363 h 9240982"/>
+            <a:gd name="connsiteX6" fmla="*/ 2549237 w 2645420"/>
+            <a:gd name="connsiteY6" fmla="*/ 1316182 h 9240982"/>
+            <a:gd name="connsiteX7" fmla="*/ 2604655 w 2645420"/>
+            <a:gd name="connsiteY7" fmla="*/ 1634836 h 9240982"/>
+            <a:gd name="connsiteX8" fmla="*/ 2618509 w 2645420"/>
+            <a:gd name="connsiteY8" fmla="*/ 3477491 h 9240982"/>
+            <a:gd name="connsiteX9" fmla="*/ 2563091 w 2645420"/>
+            <a:gd name="connsiteY9" fmla="*/ 3865418 h 9240982"/>
+            <a:gd name="connsiteX10" fmla="*/ 2410691 w 2645420"/>
+            <a:gd name="connsiteY10" fmla="*/ 4391891 h 9240982"/>
+            <a:gd name="connsiteX11" fmla="*/ 2022764 w 2645420"/>
+            <a:gd name="connsiteY11" fmla="*/ 5167745 h 9240982"/>
+            <a:gd name="connsiteX12" fmla="*/ 1759528 w 2645420"/>
+            <a:gd name="connsiteY12" fmla="*/ 5611091 h 9240982"/>
+            <a:gd name="connsiteX13" fmla="*/ 1704109 w 2645420"/>
+            <a:gd name="connsiteY13" fmla="*/ 5791200 h 9240982"/>
+            <a:gd name="connsiteX14" fmla="*/ 1468582 w 2645420"/>
+            <a:gd name="connsiteY14" fmla="*/ 6206836 h 9240982"/>
+            <a:gd name="connsiteX15" fmla="*/ 1371600 w 2645420"/>
+            <a:gd name="connsiteY15" fmla="*/ 6622472 h 9240982"/>
+            <a:gd name="connsiteX16" fmla="*/ 1316182 w 2645420"/>
+            <a:gd name="connsiteY16" fmla="*/ 6830291 h 9240982"/>
+            <a:gd name="connsiteX17" fmla="*/ 1260764 w 2645420"/>
+            <a:gd name="connsiteY17" fmla="*/ 7093527 h 9240982"/>
+            <a:gd name="connsiteX18" fmla="*/ 1108364 w 2645420"/>
+            <a:gd name="connsiteY18" fmla="*/ 7426036 h 9240982"/>
+            <a:gd name="connsiteX19" fmla="*/ 1025237 w 2645420"/>
+            <a:gd name="connsiteY19" fmla="*/ 7744691 h 9240982"/>
+            <a:gd name="connsiteX20" fmla="*/ 983673 w 2645420"/>
+            <a:gd name="connsiteY20" fmla="*/ 8174182 h 9240982"/>
+            <a:gd name="connsiteX21" fmla="*/ 845128 w 2645420"/>
+            <a:gd name="connsiteY21" fmla="*/ 8700654 h 9240982"/>
+            <a:gd name="connsiteX22" fmla="*/ 789709 w 2645420"/>
+            <a:gd name="connsiteY22" fmla="*/ 8991600 h 9240982"/>
+            <a:gd name="connsiteX23" fmla="*/ 775855 w 2645420"/>
+            <a:gd name="connsiteY23" fmla="*/ 9240982 h 9240982"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX0" y="connsiteY0"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX1" y="connsiteY1"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX2" y="connsiteY2"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX3" y="connsiteY3"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX4" y="connsiteY4"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX5" y="connsiteY5"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX6" y="connsiteY6"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX7" y="connsiteY7"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX8" y="connsiteY8"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX9" y="connsiteY9"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX10" y="connsiteY10"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX11" y="connsiteY11"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX12" y="connsiteY12"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX13" y="connsiteY13"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX14" y="connsiteY14"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX15" y="connsiteY15"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX16" y="connsiteY16"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX17" y="connsiteY17"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX18" y="connsiteY18"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX19" y="connsiteY19"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX20" y="connsiteY20"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX21" y="connsiteY21"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX22" y="connsiteY22"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX23" y="connsiteY23"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="2645420" h="9240982">
+              <a:moveTo>
+                <a:pt x="0" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="997528" y="180109"/>
+              </a:lnTo>
+              <a:cubicBezTo>
+                <a:pt x="1081203" y="195914"/>
+                <a:pt x="1167950" y="203640"/>
+                <a:pt x="1246909" y="235527"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1586222" y="372557"/>
+                <a:pt x="1702450" y="444751"/>
+                <a:pt x="1953491" y="651163"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2085043" y="759328"/>
+                <a:pt x="2215873" y="868589"/>
+                <a:pt x="2341418" y="983672"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2382411" y="1021249"/>
+                <a:pt x="2422782" y="1061205"/>
+                <a:pt x="2452255" y="1108363"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2492771" y="1173188"/>
+                <a:pt x="2516910" y="1246909"/>
+                <a:pt x="2549237" y="1316182"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2567710" y="1422400"/>
+                <a:pt x="2590406" y="1527969"/>
+                <a:pt x="2604655" y="1634836"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2679196" y="2193893"/>
+                <a:pt x="2631174" y="3125399"/>
+                <a:pt x="2618509" y="3477491"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2613813" y="3608028"/>
+                <a:pt x="2585954" y="3736813"/>
+                <a:pt x="2563091" y="3865418"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2535073" y="4023019"/>
+                <a:pt x="2468770" y="4249332"/>
+                <a:pt x="2410691" y="4391891"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2282719" y="4706005"/>
+                <a:pt x="2190254" y="4888596"/>
+                <a:pt x="2022764" y="5167745"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1956807" y="5277674"/>
+                <a:pt x="1815889" y="5467058"/>
+                <a:pt x="1759528" y="5611091"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1736639" y="5669586"/>
+                <a:pt x="1733771" y="5735831"/>
+                <a:pt x="1704109" y="5791200"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1478795" y="6211784"/>
+                <a:pt x="1608620" y="5786721"/>
+                <a:pt x="1468582" y="6206836"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1406548" y="6392939"/>
+                <a:pt x="1415808" y="6433011"/>
+                <a:pt x="1371600" y="6622472"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1355309" y="6692290"/>
+                <a:pt x="1332603" y="6760503"/>
+                <a:pt x="1316182" y="6830291"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1295644" y="6917576"/>
+                <a:pt x="1290298" y="7008862"/>
+                <a:pt x="1260764" y="7093527"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1220606" y="7208647"/>
+                <a:pt x="1139140" y="7308061"/>
+                <a:pt x="1108364" y="7426036"/>
+              </a:cubicBezTo>
+              <a:lnTo>
+                <a:pt x="1025237" y="7744691"/>
+              </a:lnTo>
+              <a:cubicBezTo>
+                <a:pt x="1011382" y="7887855"/>
+                <a:pt x="1029157" y="8037731"/>
+                <a:pt x="983673" y="8174182"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="914443" y="8381873"/>
+                <a:pt x="928367" y="8333016"/>
+                <a:pt x="845128" y="8700654"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="823327" y="8796942"/>
+                <a:pt x="802263" y="8893676"/>
+                <a:pt x="789709" y="8991600"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="779122" y="9074180"/>
+                <a:pt x="780473" y="9157855"/>
+                <a:pt x="775855" y="9240982"/>
+              </a:cubicBezTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-PH" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2824,8 +6212,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{529E1EE1-84BC-44E9-9DB6-5CF40692FF92}">
   <dimension ref="B1:R61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView topLeftCell="A42" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="M68" sqref="M68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2920,10 +6308,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AEB8265-3C8E-4609-81CC-B5279E8DC9E7}">
-  <dimension ref="A2:B2"/>
+  <dimension ref="A2:R48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="Y64" sqref="Y64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2934,7 +6322,28 @@
         <v>2</v>
       </c>
     </row>
+    <row r="28" spans="14:14" x14ac:dyDescent="0.3">
+      <c r="N28" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="11:18" x14ac:dyDescent="0.3">
+      <c r="R38" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="11:18" x14ac:dyDescent="0.3">
+      <c r="K39" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="11:18" x14ac:dyDescent="0.3">
+      <c r="N48" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
i fogot added illustration schematic
</commit_message>
<xml_diff>
--- a/Generator/2dparts_schematic_materials-gen.xlsx
+++ b/Generator/2dparts_schematic_materials-gen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\school\2ndyr\1stsem\emag\generotr\Generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{139083B3-6BC9-41B6-94A4-818743CB9452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32198340-3A5C-4B4C-8108-C68555FAC4A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{6EB7C18F-EE50-4A76-837B-874021D0598F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6EB7C18F-EE50-4A76-837B-874021D0598F}"/>
   </bookViews>
   <sheets>
     <sheet name="General Schematic" sheetId="2" r:id="rId1"/>
@@ -6212,7 +6212,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{529E1EE1-84BC-44E9-9DB6-5CF40692FF92}">
   <dimension ref="B1:R61"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="M68" sqref="M68"/>
     </sheetView>
   </sheetViews>
@@ -6310,7 +6310,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AEB8265-3C8E-4609-81CC-B5279E8DC9E7}">
   <dimension ref="A2:R48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="Y64" sqref="Y64"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added schematic of the controller
</commit_message>
<xml_diff>
--- a/Generator/2dparts_schematic_materials-gen.xlsx
+++ b/Generator/2dparts_schematic_materials-gen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\school\2ndyr\1stsem\emag\generotr\Generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32198340-3A5C-4B4C-8108-C68555FAC4A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AD0869D-8525-441A-BBE6-F3328B91891B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6EB7C18F-EE50-4A76-837B-874021D0598F}"/>
   </bookViews>
@@ -458,7 +458,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-PH" sz="1100" baseline="0"/>
-            <a:t> Ah</a:t>
+            <a:t> Ah 2C</a:t>
           </a:r>
           <a:endParaRPr lang="en-PH" sz="1100"/>
         </a:p>
@@ -484,16 +484,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>79</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>385482</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>58719</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>388620</xdr:colOff>
-      <xdr:row>83</xdr:row>
-      <xdr:rowOff>144780</xdr:rowOff>
+      <xdr:colOff>164502</xdr:colOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>1345</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -508,8 +508,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4480560" y="6972300"/>
-          <a:ext cx="998220" cy="853440"/>
+          <a:off x="4258235" y="9561307"/>
+          <a:ext cx="998220" cy="839097"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -786,15 +786,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>388620</xdr:colOff>
-      <xdr:row>81</xdr:row>
-      <xdr:rowOff>83820</xdr:rowOff>
+      <xdr:colOff>164502</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>119680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>121920</xdr:colOff>
-      <xdr:row>81</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
+      <xdr:colOff>215153</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>161365</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -811,8 +811,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="5478780" y="7399020"/>
-          <a:ext cx="342900" cy="15240"/>
+          <a:off x="5256455" y="9980856"/>
+          <a:ext cx="660251" cy="41685"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -993,16 +993,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>274320</xdr:colOff>
-      <xdr:row>83</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>41238</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>21515</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>327660</xdr:colOff>
-      <xdr:row>96</xdr:row>
-      <xdr:rowOff>83820</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>94578</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>74854</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1017,8 +1017,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="274320" y="7711440"/>
-          <a:ext cx="2705100" cy="2430780"/>
+          <a:off x="650838" y="6834691"/>
+          <a:ext cx="2706893" cy="2384163"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -1058,94 +1058,12 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="en-PH" sz="1100"/>
-            <a:t>5v (256 leds)</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-PH" sz="1100"/>
-            <a:t>max/px</a:t>
+            <a:t>5V</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-PH" sz="1100" baseline="0"/>
-            <a:t> = </a:t>
+            <a:t> </a:t>
           </a:r>
-          <a:r>
-            <a:rPr lang="en-PH" sz="1100"/>
-            <a:t>(0.2W / px)</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-PH" sz="1100"/>
-            <a:t>max total px = 51.2W</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-PH" sz="1100"/>
-            <a:t>current/px</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-PH" sz="1100" baseline="0"/>
-            <a:t> =  40mA</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-PH" sz="1100" baseline="0"/>
-            <a:t>max total current = 10.24A</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-PH" sz="1100"/>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-PH" sz="1100"/>
-            <a:t>if one color</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-PH" sz="1100" baseline="0"/>
-            <a:t> only:</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-PH" sz="1100" baseline="0"/>
-            <a:t>max/px = 0.0666667W / px</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-PH" sz="1100" baseline="0"/>
-            <a:t>max total px = 17.0667W</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-PH" sz="1100" baseline="0"/>
-            <a:t>current/px = 13.333mA</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-PH" sz="1100" baseline="0"/>
-            <a:t>max total current = 3.4144A</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
           <a:endParaRPr lang="en-PH" sz="1100"/>
         </a:p>
       </xdr:txBody>
@@ -1154,16 +1072,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>350520</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>94578</xdr:colOff>
       <xdr:row>85</xdr:row>
       <xdr:rowOff>137160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>86</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>137832</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1174,12 +1092,14 @@
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="47" idx="3"/>
+        </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="3002280" y="8183880"/>
-          <a:ext cx="3116580" cy="68580"/>
+          <a:off x="3357731" y="8026101"/>
+          <a:ext cx="2762922" cy="672"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1194,108 +1114,6 @@
         </a:fillRef>
         <a:effectRef idx="2">
           <a:schemeClr val="accent6"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>464820</xdr:colOff>
-      <xdr:row>67</xdr:row>
-      <xdr:rowOff>129540</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>464820</xdr:colOff>
-      <xdr:row>72</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="51" name="Straight Connector 50">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25430925-7401-302F-90AE-C6C4862DAC76}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1074420" y="4884420"/>
-          <a:ext cx="0" cy="861060"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="accent2"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent2"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent2"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>255270</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>72</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="54" name="Straight Connector 53">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{98E6E759-5C0C-0F07-311D-A8DF71949BAD}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:endCxn id="94" idx="0"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="2907030" y="5151120"/>
-          <a:ext cx="11430" cy="556260"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="dk1"/>
         </a:effectRef>
         <a:fontRef idx="minor">
           <a:schemeClr val="tx1"/>
@@ -1437,15 +1255,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
+      <xdr:colOff>129540</xdr:colOff>
       <xdr:row>70</xdr:row>
       <xdr:rowOff>7620</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>129540</xdr:colOff>
-      <xdr:row>81</xdr:row>
-      <xdr:rowOff>83820</xdr:rowOff>
+      <xdr:colOff>206188</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>161365</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1459,9 +1277,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="5814060" y="5311140"/>
-          <a:ext cx="15240" cy="2087880"/>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="5831093" y="5207149"/>
+          <a:ext cx="76648" cy="4815392"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1588,14 +1406,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>601980</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>548192</xdr:colOff>
       <xdr:row>72</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>35859</xdr:colOff>
       <xdr:row>74</xdr:row>
       <xdr:rowOff>175260</xdr:rowOff>
     </xdr:to>
@@ -1612,8 +1430,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2034540" y="5707380"/>
-          <a:ext cx="1531620" cy="502920"/>
+          <a:off x="1157792" y="5596218"/>
+          <a:ext cx="1531620" cy="495748"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -1666,110 +1484,10 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>716280</xdr:colOff>
-      <xdr:row>74</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>731520</xdr:colOff>
-      <xdr:row>83</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="103" name="Straight Connector 102">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{39050B76-BFA7-2664-03CD-353BD19F474C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1325880" y="6210300"/>
-          <a:ext cx="15240" cy="1562100"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>434340</xdr:colOff>
-      <xdr:row>74</xdr:row>
-      <xdr:rowOff>53340</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>510540</xdr:colOff>
-      <xdr:row>83</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="105" name="Straight Connector 104">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{35C6AC23-3E54-1B95-9013-F4C17F4F62AF}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1043940" y="6088380"/>
-          <a:ext cx="76200" cy="1744980"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="accent2"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent2"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent2"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>35859</xdr:colOff>
       <xdr:row>73</xdr:row>
-      <xdr:rowOff>49530</xdr:rowOff>
+      <xdr:rowOff>51323</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
@@ -1793,8 +1511,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="3566160" y="5901690"/>
-          <a:ext cx="6416040" cy="57150"/>
+          <a:off x="2689412" y="5788735"/>
+          <a:ext cx="7294581" cy="55357"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1820,15 +1538,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>499110</xdr:colOff>
-      <xdr:row>73</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>274992</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>71718</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>510540</xdr:colOff>
-      <xdr:row>79</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
+      <xdr:colOff>358588</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>58719</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1845,8 +1563,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="4979670" y="5928360"/>
-          <a:ext cx="11430" cy="1043940"/>
+          <a:off x="4757345" y="5988424"/>
+          <a:ext cx="83596" cy="3572883"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1921,8 +1639,8 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>591671</xdr:colOff>
       <xdr:row>74</xdr:row>
       <xdr:rowOff>7620</xdr:rowOff>
     </xdr:from>
@@ -1930,7 +1648,7 @@
       <xdr:col>16</xdr:col>
       <xdr:colOff>22860</xdr:colOff>
       <xdr:row>74</xdr:row>
-      <xdr:rowOff>45720</xdr:rowOff>
+      <xdr:rowOff>71718</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1945,8 +1663,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="3566160" y="6042660"/>
-          <a:ext cx="6423660" cy="38100"/>
+          <a:off x="2635624" y="5924326"/>
+          <a:ext cx="7355989" cy="64098"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1972,15 +1690,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>53340</xdr:colOff>
+      <xdr:colOff>18316</xdr:colOff>
       <xdr:row>74</xdr:row>
       <xdr:rowOff>45720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>68580</xdr:colOff>
-      <xdr:row>79</xdr:row>
-      <xdr:rowOff>83820</xdr:rowOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>2308</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1991,12 +1709,14 @@
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="17" idx="7"/>
+        </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="5143500" y="6080760"/>
-          <a:ext cx="15240" cy="952500"/>
+          <a:off x="5110269" y="5962426"/>
+          <a:ext cx="50264" cy="3721764"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2137,15 +1857,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>373380</xdr:colOff>
+      <xdr:colOff>402964</xdr:colOff>
       <xdr:row>63</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>403860</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:colOff>489249</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2158,12 +1878,13 @@
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="14" idx="2"/>
+          <a:endCxn id="94" idx="0"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="1805940" y="4145280"/>
-          <a:ext cx="30480" cy="800100"/>
+        <a:xfrm>
+          <a:off x="1837317" y="4066391"/>
+          <a:ext cx="86285" cy="1529827"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2194,10 +1915,10 @@
       <xdr:rowOff>137160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>594360</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>68580</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>8965</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>35858</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2212,8 +1933,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2019300" y="4160520"/>
-          <a:ext cx="7620" cy="1028700"/>
+          <a:off x="2021093" y="4081631"/>
+          <a:ext cx="31825" cy="1512345"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2238,32 +1959,32 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>708660</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>358588</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>64545</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>297180</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>26446</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>89647</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="150" name="Straight Connector 149">
+        <xdr:cNvPr id="50" name="Straight Connector 49">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{646D462F-BCB9-08E3-9B63-732CDC26509E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{593E1216-AFD5-8D4D-360C-A06202A9EF62}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="1318260" y="5143500"/>
-          <a:ext cx="1630680" cy="15240"/>
+        <a:xfrm flipH="1">
+          <a:off x="1792941" y="6519133"/>
+          <a:ext cx="2106258" cy="25102"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2288,294 +2009,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>449580</xdr:colOff>
-      <xdr:row>67</xdr:row>
-      <xdr:rowOff>121920</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>129540</xdr:colOff>
-      <xdr:row>67</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="151" name="Straight Connector 150">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD21FA15-2251-82FE-2700-D1B412CDB6B8}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1059180" y="4876800"/>
-          <a:ext cx="1722120" cy="30480"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="accent2"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent2"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent2"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>320040</xdr:colOff>
-      <xdr:row>72</xdr:row>
-      <xdr:rowOff>60960</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>75</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="Rectangle: Rounded Corners 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{321C48DB-C23F-731C-DF18-CC9F904DC7ED}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="320040" y="5730240"/>
-          <a:ext cx="1531620" cy="502920"/>
-        </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent4">
-            <a:shade val="15000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent4"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent4"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-PH" sz="1100"/>
-            <a:t>buck converter</a:t>
-          </a:r>
-          <a:br>
-            <a:rPr lang="en-PH" sz="1100"/>
-          </a:br>
-          <a:r>
-            <a:rPr lang="en-PH" sz="1100"/>
-            <a:t>(output: </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-PH" sz="1100" baseline="0"/>
-            <a:t>5v; max 5-6A</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-PH" sz="1100"/>
-            <a:t>)</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>83820</xdr:colOff>
-      <xdr:row>67</xdr:row>
-      <xdr:rowOff>144780</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>72</xdr:row>
-      <xdr:rowOff>45720</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="6" name="Straight Connector 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79D52673-6F2C-1C5E-F66F-883DEF6AD3BE}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="2735580" y="4899660"/>
-          <a:ext cx="30480" cy="815340"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="accent2"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent2"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent2"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>681990</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>53340</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>693420</xdr:colOff>
-      <xdr:row>72</xdr:row>
-      <xdr:rowOff>60960</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="7" name="Straight Connector 6">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D55E1D2-2AA6-4157-8B2D-959D87A64EFE}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="1291590" y="5173980"/>
-          <a:ext cx="11430" cy="556260"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>701040</xdr:colOff>
-      <xdr:row>79</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>53340</xdr:colOff>
-      <xdr:row>79</xdr:row>
-      <xdr:rowOff>129540</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="50" name="Straight Connector 49">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{593E1216-AFD5-8D4D-360C-A06202A9EF62}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="1310640" y="7040880"/>
-          <a:ext cx="2613660" cy="38100"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>472440</xdr:colOff>
-      <xdr:row>78</xdr:row>
-      <xdr:rowOff>129540</xdr:rowOff>
+      <xdr:colOff>17930</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>84716</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>487680</xdr:colOff>
-      <xdr:row>78</xdr:row>
-      <xdr:rowOff>144780</xdr:rowOff>
+      <xdr:colOff>469751</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>116541</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2590,8 +2033,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="1082040" y="6896100"/>
-          <a:ext cx="2667000" cy="15240"/>
+          <a:off x="1452283" y="6360010"/>
+          <a:ext cx="2280621" cy="31825"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2617,15 +2060,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
+      <xdr:colOff>26894</xdr:colOff>
       <xdr:row>74</xdr:row>
       <xdr:rowOff>45720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>60960</xdr:colOff>
-      <xdr:row>79</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>62753</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2639,9 +2082,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3909060" y="6080760"/>
-          <a:ext cx="22860" cy="982980"/>
+        <a:xfrm flipH="1">
+          <a:off x="3899647" y="5962426"/>
+          <a:ext cx="11206" cy="554915"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2667,15 +2110,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>449580</xdr:colOff>
+      <xdr:colOff>448235</xdr:colOff>
       <xdr:row>73</xdr:row>
       <xdr:rowOff>106680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>78</xdr:row>
-      <xdr:rowOff>129540</xdr:rowOff>
+      <xdr:colOff>449580</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>80682</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2689,9 +2132,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3710940" y="5958840"/>
-          <a:ext cx="7620" cy="937260"/>
+        <a:xfrm flipH="1">
+          <a:off x="3711388" y="5844092"/>
+          <a:ext cx="1345" cy="511884"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2784,17 +2227,9 @@
         <a:p>
           <a:pPr algn="l"/>
           <a:r>
-            <a:rPr lang="en-PH" sz="1100"/>
-            <a:t>6.8</a:t>
+            <a:rPr lang="en-PH" sz="1100" baseline="0"/>
+            <a:t>2.4 Ah (2S) </a:t>
           </a:r>
-          <a:r>
-            <a:rPr lang="en-PH" sz="1100" baseline="0"/>
-            <a:t> Ah (2S)</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-PH" sz="1100"/>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
           <a:endParaRPr lang="en-PH" sz="1100"/>
         </a:p>
         <a:p>
@@ -2807,6 +2242,106 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>358588</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>53789</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>385482</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="15" name="Straight Connector 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE437855-85C8-1ADF-EAD4-41854F184B38}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1792941" y="6508377"/>
+          <a:ext cx="26894" cy="304799"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>62753</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>89647</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>71718</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>89648</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="Straight Connector 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DDD47B8B-580C-7B4C-6F0E-17C025E10B01}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1497106" y="6364941"/>
+          <a:ext cx="8965" cy="537883"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -6212,8 +5747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{529E1EE1-84BC-44E9-9DB6-5CF40692FF92}">
   <dimension ref="B1:R61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="M68" sqref="M68"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P90" sqref="P90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6310,7 +5845,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AEB8265-3C8E-4609-81CC-B5279E8DC9E7}">
   <dimension ref="A2:R48"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="Y64" sqref="Y64"/>
     </sheetView>
   </sheetViews>

</xml_diff>